<commit_message>
Fuel-Flow to Load Test Testcase Run Completed
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\Tickets\EASEY-94 QA Test Case Scripting\CaseResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC34352-DF62-4A7C-BE01-626113BECAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57293870-0167-4A78-A821-4797FEC5DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="Linearity Cases" sheetId="1" r:id="rId1"/>
     <sheet name="RATA Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Fuel-Flow To Load Test Cases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5782" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6018" uniqueCount="831">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -2371,6 +2372,165 @@
   </si>
   <si>
     <t>QAT "MDC-F33C839459EE443ABBE35920852434DD" "TGOSQL12SV-AD19AE8813B0455CAE544E0F2AA0102F"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES1-A</t>
+  </si>
+  <si>
+    <t>FF2LTST</t>
+  </si>
+  <si>
+    <t>FF2L-Q32021-01A-1</t>
+  </si>
+  <si>
+    <t>01A (CO2)</t>
+  </si>
+  <si>
+    <t>FF2LTST-1-B</t>
+  </si>
+  <si>
+    <t>According to the monitoring system record, the monitoring system for this fuel flow-to-load test was not a fuel flow system.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F3ED630C7DE34EFA8BB22A34B636F88B" "NC-PORTERK-2C6905A0FC1245B8BC2358A8262E71F8"</t>
+  </si>
+  <si>
+    <t>FF2LTST-2-C</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES1-B</t>
+  </si>
+  <si>
+    <t>FF2L-Q12019-02A-2</t>
+  </si>
+  <si>
+    <t>02A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LTST-11-A</t>
+  </si>
+  <si>
+    <t>You did not provide TestResultCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-6D401A983DDA4D919F2B6EC67DB6E651"</t>
+  </si>
+  <si>
+    <t>FF2L-Q12020-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-7-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedCofiring for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-0BAEAEC0BC024BF0B46489F9EB39D613"</t>
+  </si>
+  <si>
+    <t>FF2L-Q12021-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-5-E</t>
+  </si>
+  <si>
+    <t>The TestResultCode of the fuel flow-to-load test indicates a failing test, but the AverageDifference indicates a passing test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-2E18521EDF874146996237F7184208FC"</t>
+  </si>
+  <si>
+    <t>FF2LTST-6-C</t>
+  </si>
+  <si>
+    <t>The NumberOfHoursUsed was less than 168 which is the minimum required to complete the quarterly fuel flow-to-load test.</t>
+  </si>
+  <si>
+    <t>FF2L-Q22019-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-10-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-D1D6E2A3226449298D5F78B51BC674EF"</t>
+  </si>
+  <si>
+    <t>FF2L-Q22020-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-4-B</t>
+  </si>
+  <si>
+    <t>The TestBasisCode is inconsistent with the data submitted in the associated fuel flow-to-load baseline data.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-E06718BEF23B45F7BB7163593FF55571"</t>
+  </si>
+  <si>
+    <t>FF2L-Q22021-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-3-A</t>
+  </si>
+  <si>
+    <t>You did not provide TestBasisCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-9EBE9F31F97A40B4A550E6ADFC3BB93E"</t>
+  </si>
+  <si>
+    <t>FF2L-Q32019-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-9-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedLowRange for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-15CC64B2F83B450D88C2ED86BB1CD36C"</t>
+  </si>
+  <si>
+    <t>FF2L-Q32021-02A-2</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-FDA53799F10F4AAFA43AF220712AFBF8"</t>
+  </si>
+  <si>
+    <t>FF2L-Q42018-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-12-A</t>
+  </si>
+  <si>
+    <t>The total number of hours used in the fuel flow-to-load or GHR analysis and the number of hours excluded exceed the total number of hours in the quarter.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-68AAAFBB42A1472BA590A2A55FB26855"</t>
+  </si>
+  <si>
+    <t>FF2L-Q42019-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-8-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedRamping for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-F106F030CEEF492EA479A9DEC6DB5028"</t>
+  </si>
+  <si>
+    <t>FF2L-Q42020-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LTST-6-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursUsed for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-A137227A737345E6BA99604C9FC5E3B8"</t>
   </si>
 </sst>
 </file>
@@ -2455,7 +2615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2490,11 +2650,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="40">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2624,39 +2865,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4972,11 +5233,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF247E8-4CEE-4E4C-AA1C-A5F6418303B4}">
   <dimension ref="A1:K581"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4990,7 +5251,7 @@
     <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="64.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="56.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="41.28515625" style="5" customWidth="1"/>
     <col min="11" max="11" width="104.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -23611,4 +23872,798 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="61.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="98.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fuel-Flow to Load Test Case Run Completion
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57293870-0167-4A78-A821-4797FEC5DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A844C02D-C64B-4A87-8900-596E9E342505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="Linearity Cases" sheetId="1" r:id="rId1"/>
     <sheet name="RATA Cases" sheetId="2" r:id="rId2"/>
-    <sheet name="Fuel-Flow To Load Test Cases" sheetId="3" r:id="rId3"/>
+    <sheet name="FuelFlow To Load Test Cases" sheetId="3" r:id="rId3"/>
+    <sheet name="FuelFlow To Load Baseline Cases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6018" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="922">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -2531,6 +2532,279 @@
   </si>
   <si>
     <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-A137227A737345E6BA99604C9FC5E3B8"</t>
+  </si>
+  <si>
+    <t>FF2LBAS</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-01A-1</t>
+  </si>
+  <si>
+    <t>FF2LBAS-1-B</t>
+  </si>
+  <si>
+    <t>According to the monitoring system record, the monitoring system for this fuel flow-to-load baseline data record was not a fuel flow system.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F3ED630C7DE34EFA8BB22A34B636F88B" "NC-PORTERK-BDDB557D060C41B8969061D494D92A5C"</t>
+  </si>
+  <si>
+    <t>FF2LBAS-2-C</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-02A-2</t>
+  </si>
+  <si>
+    <t>FF2LBAS-3-A</t>
+  </si>
+  <si>
+    <t>You did not provide AccuracyTestNumber, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-DADB116D7B074BBAB722F6842F5ADA6B"</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-02A-2</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9D275D287FBF42CAAECBECA1A097558D" "NC-PORTERK-1C3822E0E2124707BB31B767BC51B2C3"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES2-A</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-03A-5</t>
+  </si>
+  <si>
+    <t>03A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-14-B</t>
+  </si>
+  <si>
+    <t>The number of hours excluded in the baseline data collection period exceeds the number of available clock hours in the period.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-59DA9CEF8EFF42C1B0AE839A5EC7CE35" "NC-PORTERK-C72C82072C444CC79E2F57B6124ED59C"</t>
+  </si>
+  <si>
+    <t>FF2LBAS-5-A</t>
+  </si>
+  <si>
+    <t>The baseline period exceeds the 4 quarters allowed for the collection of fuel flow-to-load baseline data.</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-03A-5</t>
+  </si>
+  <si>
+    <t>FF2LBAS-4-A</t>
+  </si>
+  <si>
+    <t>You reported both a Fuel flow-to-load ratio and a GHR value.  Since only one methodology can be used, this record is invalid.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-59DA9CEF8EFF42C1B0AE839A5EC7CE35" "NC-PORTERK-129B38F099274B80A7053461D8763BA9"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES2-B</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-04A-6</t>
+  </si>
+  <si>
+    <t>04A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-7-A</t>
+  </si>
+  <si>
+    <t>You did not provide AverageLoad, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F163EC790F8540589B19A3DA0E8BF3B0" "NC-PORTERK-B224AD762EDB46118555F0DFE79DFFF2"</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-04A-6</t>
+  </si>
+  <si>
+    <t>FF2LBAS-6-B</t>
+  </si>
+  <si>
+    <t>The test identified by the PEITestNumber in the fuel flow-to-load baseline data cannot be found.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F163EC790F8540589B19A3DA0E8BF3B0" "NC-PORTERK-AD7CCF5164084E51AC978D4899FFB061"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES3-A</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-05A-9</t>
+  </si>
+  <si>
+    <t>05A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-8-A</t>
+  </si>
+  <si>
+    <t>You defined an invalid AverageHourlyHeatInputRate for this test.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-88DF03257BEB4259A84C621191CD3E90" "NC-PORTERK-F18881D9C17B4853A1310E83776B98F6"</t>
+  </si>
+  <si>
+    <t>FF2LBAS-16-A</t>
+  </si>
+  <si>
+    <t>You did not provide GHRUnitsOfMeasureCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>FF2LBAS-18-A</t>
+  </si>
+  <si>
+    <t>You did not provide BaselineGHR, which is required for this test.</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES3-B</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-06A-10</t>
+  </si>
+  <si>
+    <t>06A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-9-B</t>
+  </si>
+  <si>
+    <t>The AverageHourlyHeatInputRate for the baseline period exceeds the maximum heat input capacity for the unit or for all units linked to the pipe.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9CAF43DE147D4B728E55A78C7CD13A6B" "NC-PORTERK-549BA80F41EB4783BD70FA9DE2B4F81A"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES4-A</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-07A-13</t>
+  </si>
+  <si>
+    <t>07A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-10-A</t>
+  </si>
+  <si>
+    <t>You defined an invalid AverageFuelFlowRate for this test.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-881AA62E471C4F6D86B1C9CF15F9224C" "NC-PORTERK-ADBD6ABAB40542D9B1961F0DF8730411"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES4-B</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-08A-14</t>
+  </si>
+  <si>
+    <t>08A (GAS)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-9B42B3CE6D7D4F95BD48D5B8413C0FF3" "NC-PORTERK-7F4B3EA6893A42D895ACD7B80D3BDAE3"</t>
+  </si>
+  <si>
+    <t>FF2LBAS-11-A</t>
+  </si>
+  <si>
+    <t>According to the Accuracy Test (and PEI) associated with the fuel flow-to-load baseline data, the begin date and hour of the baseline data collection period is prior to the date when the accuracy test (and PEI) were completed or the flowmeter was reinstalled.</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES5-A</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-09A-17</t>
+  </si>
+  <si>
+    <t>09A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-12-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-72022806AF864AA0BFB5F772EEAE433D" "NC-PORTERK-5DDDEFAB27104DFFA5277B0E38998B18"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES5-B</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-10A-18</t>
+  </si>
+  <si>
+    <t>10A (GAS)</t>
+  </si>
+  <si>
+    <t>FF2LBAS-14-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-6C8FC79314A94DE6973CE3CE0ED87F64" "NC-PORTERK-7D05BA490C0F4F12BD9C5A40EC1EA5DE"</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-10A-18</t>
+  </si>
+  <si>
+    <t>FF2LBAS-13-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-6C8FC79314A94DE6973CE3CE0ED87F64" "NC-PORTERK-DBC1D8DD91F24F82BEE575A32487143E"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES6-A</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-11A-21</t>
+  </si>
+  <si>
+    <t>11A (GAS)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-C00BECCBFFBF4447A2AD4F5C0AD78D3E" "NC-PORTERK-A6CBBF6E5D704B58B44C02B4B0479131"</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-11A-21</t>
+  </si>
+  <si>
+    <t>FF2LBAS-15-A</t>
+  </si>
+  <si>
+    <t>You did not provide FuelFlowToLoadUOMCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-C00BECCBFFBF4447A2AD4F5C0AD78D3E" "NC-PORTERK-2BE5688CCFFE4D9FA679FAA5E8E058EC"</t>
+  </si>
+  <si>
+    <t>ORIS 56249 (NCEMC Anson Plant) Location ES6-B</t>
+  </si>
+  <si>
+    <t>FF2B-Q32016-12A-22</t>
+  </si>
+  <si>
+    <t>12A (GAS)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F29B1E823FF24AD490BBFEE45079B809" "NC-PORTERK-068C3936ABD442EF84D1CF8999AD9E38"</t>
+  </si>
+  <si>
+    <t>FF2B-Q32021-12A-22</t>
+  </si>
+  <si>
+    <t>FF2LBAS-17-B</t>
+  </si>
+  <si>
+    <t>You defined an invalid BaselineFuelFlowToLoadRatio for this test.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-F29B1E823FF24AD490BBFEE45079B809" "NC-PORTERK-C2BA677FE85D4E89B017D1D0CEAD1809"</t>
   </si>
 </sst>
 </file>
@@ -2615,7 +2889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2650,26 +2924,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <font>
         <b/>
@@ -2706,6 +2965,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2722,6 +2996,49 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2865,59 +3182,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="0" dataDxfId="26" headerRowBorderDxfId="27">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="14">
+  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23878,11 +24215,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23900,11 +24237,803 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A12ED-21A8-440D-BCEA-B358D4E41F2C}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="41.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="98.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -23916,13 +25045,13 @@
       <c r="E1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="8" t="s">
         <v>94</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -23940,10 +25069,10 @@
         <v>778</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>780</v>
+        <v>832</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>781</v>
@@ -23952,16 +25081,16 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>782</v>
+        <v>833</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>783</v>
+        <v>834</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>784</v>
+        <v>835</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -23969,10 +25098,10 @@
         <v>778</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>780</v>
+        <v>832</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>781</v>
@@ -23981,7 +25110,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>785</v>
+        <v>836</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>94</v>
@@ -23990,7 +25119,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>784</v>
+        <v>835</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -23998,10 +25127,10 @@
         <v>786</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>787</v>
+        <v>837</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>788</v>
@@ -24010,16 +25139,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>789</v>
+        <v>838</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>790</v>
+        <v>839</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>791</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -24027,10 +25156,10 @@
         <v>786</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>787</v>
+        <v>837</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>788</v>
@@ -24039,7 +25168,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>785</v>
+        <v>836</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>94</v>
@@ -24048,7 +25177,7 @@
         <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>791</v>
+        <v>840</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -24056,396 +25185,396 @@
         <v>786</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>792</v>
+        <v>841</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>788</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>793</v>
+        <v>836</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>794</v>
+        <v>16</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>795</v>
+        <v>842</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>786</v>
+        <v>843</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>792</v>
+        <v>844</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>788</v>
+        <v>845</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>785</v>
+        <v>846</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>16</v>
+        <v>847</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>795</v>
+        <v>848</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>786</v>
+        <v>843</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>796</v>
+        <v>844</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>788</v>
+        <v>845</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>798</v>
+        <v>850</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>799</v>
+        <v>848</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>786</v>
+        <v>843</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>796</v>
+        <v>844</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>788</v>
+        <v>845</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>800</v>
+        <v>836</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>801</v>
+        <v>16</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>799</v>
+        <v>848</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>786</v>
+        <v>843</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>796</v>
+        <v>851</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>788</v>
+        <v>845</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>785</v>
+        <v>852</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>16</v>
+        <v>853</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>799</v>
+        <v>854</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>786</v>
+        <v>843</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>802</v>
+        <v>851</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>788</v>
+        <v>845</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>803</v>
+        <v>836</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>804</v>
+        <v>854</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>786</v>
+        <v>855</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>802</v>
+        <v>856</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>788</v>
+        <v>857</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>785</v>
+        <v>858</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>16</v>
+        <v>859</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>786</v>
+        <v>855</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>805</v>
+        <v>856</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>788</v>
+        <v>857</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>806</v>
+        <v>836</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>807</v>
+        <v>16</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>808</v>
+        <v>860</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>786</v>
+        <v>855</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>805</v>
+        <v>861</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>788</v>
+        <v>857</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>785</v>
+        <v>862</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>16</v>
+        <v>863</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>808</v>
+        <v>864</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>786</v>
+        <v>855</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>809</v>
+        <v>861</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>788</v>
+        <v>857</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>810</v>
+        <v>836</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>811</v>
+        <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>812</v>
+        <v>864</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>786</v>
+        <v>865</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>809</v>
+        <v>866</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>788</v>
+        <v>867</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>800</v>
+        <v>868</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>801</v>
+        <v>869</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>812</v>
+        <v>870</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>786</v>
+        <v>865</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>809</v>
+        <v>866</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>788</v>
+        <v>867</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>785</v>
+        <v>871</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>16</v>
+        <v>872</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>812</v>
+        <v>870</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>786</v>
+        <v>865</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>813</v>
+        <v>866</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>788</v>
+        <v>867</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>814</v>
+        <v>873</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>815</v>
+        <v>874</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>816</v>
+        <v>870</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>786</v>
+        <v>865</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>813</v>
+        <v>866</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>788</v>
+        <v>867</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>785</v>
+        <v>836</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>94</v>
@@ -24454,210 +25583,732 @@
         <v>16</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>816</v>
+        <v>870</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>786</v>
+        <v>875</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>817</v>
+        <v>876</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>788</v>
+        <v>877</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>785</v>
+        <v>878</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>16</v>
+        <v>879</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>818</v>
+        <v>880</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>786</v>
+        <v>875</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>819</v>
+        <v>876</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>788</v>
+        <v>877</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>820</v>
+        <v>871</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>821</v>
+        <v>872</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>822</v>
+        <v>880</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>786</v>
+        <v>875</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>819</v>
+        <v>876</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>788</v>
+        <v>877</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>785</v>
+        <v>873</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>16</v>
+        <v>874</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>822</v>
+        <v>880</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>786</v>
+        <v>875</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>823</v>
+        <v>876</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>788</v>
+        <v>877</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>824</v>
+        <v>836</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>825</v>
+        <v>16</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>826</v>
+        <v>880</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>786</v>
+        <v>881</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>823</v>
+        <v>882</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>788</v>
+        <v>883</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>785</v>
+        <v>884</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>16</v>
+        <v>885</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>826</v>
+        <v>886</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>786</v>
+        <v>881</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>827</v>
+        <v>882</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>788</v>
+        <v>883</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>829</v>
+        <v>16</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>830</v>
+        <v>886</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>786</v>
+        <v>887</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>827</v>
+        <v>888</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>788</v>
+        <v>889</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>785</v>
+        <v>891</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>94</v>
       </c>
       <c r="I26" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>830</v>
+      <c r="K27" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
F2LCHK Test Case Run Completed
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD76C33F-52D2-44FA-9A72-73D1ED1F53EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BF758-7CAD-4A54-A995-FE6A56C6FB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="APPE" sheetId="6" r:id="rId1"/>
-    <sheet name="FF2LBAS" sheetId="4" r:id="rId2"/>
-    <sheet name="FF2LTST" sheetId="3" r:id="rId3"/>
-    <sheet name="LINE" sheetId="1" r:id="rId4"/>
-    <sheet name="RATA" sheetId="2" r:id="rId5"/>
-    <sheet name="UNITDEF" sheetId="5" r:id="rId6"/>
+    <sheet name="F2LCHK" sheetId="7" r:id="rId2"/>
+    <sheet name="FF2LBAS" sheetId="4" r:id="rId3"/>
+    <sheet name="FF2LTST" sheetId="3" r:id="rId4"/>
+    <sheet name="LINE" sheetId="1" r:id="rId5"/>
+    <sheet name="RATA" sheetId="2" r:id="rId6"/>
+    <sheet name="UNITDEF" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10016" uniqueCount="1298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10315" uniqueCount="1367">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -3939,6 +3940,213 @@
   </si>
   <si>
     <t>You defined an invalid OilDensity for Operating Level 1 Run Number 1 Oil System ID 100.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-D4C88AC0994340F2AB7E9E0DB1EF8FCB" "PC49096-4BA9ED868B7443D3A2FD95BE53CECBA9"</t>
+  </si>
+  <si>
+    <t>ORIS 130 (Cross) Location 1</t>
+  </si>
+  <si>
+    <t>F2LCHK</t>
+  </si>
+  <si>
+    <t>400-43</t>
+  </si>
+  <si>
+    <t>004 (FLOW)</t>
+  </si>
+  <si>
+    <t>F2LCHK-17-F</t>
+  </si>
+  <si>
+    <t>The TestResultCode is equal to "FAILED", but the AvgAbsolutePercentDiff indicates that the test passed the applicable standard based on the RATA load level reported in the flow to load reference record and the use of bias adjusted or non-adjusted values.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-0031EAFF04C74604A6AA1352D9F7372F"</t>
+  </si>
+  <si>
+    <t>F2LCHK-14-C</t>
+  </si>
+  <si>
+    <t>400-44</t>
+  </si>
+  <si>
+    <t>F2LCHK-16-A</t>
+  </si>
+  <si>
+    <t>You did not provide AvgAbsolutePercentDiff, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-22058B21D90E44AFA6B8C60ECC80D81C"</t>
+  </si>
+  <si>
+    <t>400-46</t>
+  </si>
+  <si>
+    <t>F2LCHK-15-A</t>
+  </si>
+  <si>
+    <t>You reported a TestBasisCode of H in the flow-to-load check, but the software could not find a prior flow-to-load reference data record based on the same criterion.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-73546CFACBBB45EBBF3423734D7800F8"</t>
+  </si>
+  <si>
+    <t>400-48</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-C8E5A297AC964497879CACF295A51D66"</t>
+  </si>
+  <si>
+    <t>400-50</t>
+  </si>
+  <si>
+    <t>F2LCHK-13-A</t>
+  </si>
+  <si>
+    <t>The total number of hours used in the flow-to-load or GHR analysis plus the number of hours excluded exceed the total number of hours in the quarter.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-7A00ED0D78114F288A2384AFE3C5F061"</t>
+  </si>
+  <si>
+    <t>400-53</t>
+  </si>
+  <si>
+    <t>F2LCHK-12-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcMainBypass for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-0A7E507D37E244C6B84674DCCCF9BC60"</t>
+  </si>
+  <si>
+    <t>400-54</t>
+  </si>
+  <si>
+    <t>F2LCHK-11-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedTest for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-A2EDD6C0EAFF43899BC9E788314D4644"</t>
+  </si>
+  <si>
+    <t>400-56</t>
+  </si>
+  <si>
+    <t>F2LCHK-10-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedPreRATA for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-27A9CA0C00B04163A5F75590AAD34CF8"</t>
+  </si>
+  <si>
+    <t>400-58</t>
+  </si>
+  <si>
+    <t>F2LCHK-9-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedBypass for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-AB012341DD4245DE85D743F75F132C77"</t>
+  </si>
+  <si>
+    <t>400-61</t>
+  </si>
+  <si>
+    <t>F2LCHK-8-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-F818787E16594A7595A19E4434042086"</t>
+  </si>
+  <si>
+    <t>400-63</t>
+  </si>
+  <si>
+    <t>F2LCHK-7-A</t>
+  </si>
+  <si>
+    <t>The value -1 in the field NumberOfHoursExcludedForFuel for this test is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-B47E154E104E47A0B918AAFB616AFE8D"</t>
+  </si>
+  <si>
+    <t>400-64</t>
+  </si>
+  <si>
+    <t>F2LCHK-5-A</t>
+  </si>
+  <si>
+    <t>You did not provide BiasAdjustedIndicator, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-68E349F4307A4A1E9457B6EB6E69CAED"</t>
+  </si>
+  <si>
+    <t>400-67</t>
+  </si>
+  <si>
+    <t>F2LCHK-6-C</t>
+  </si>
+  <si>
+    <t>The NumberOfHours of quality assured flow data exceeds or equals 168 hours.  A Flow-to-load analysis or GHR analysis is required for the quarter.  Do not report a TestResultCode of 'EXC168H' or 'FEW168H' for this quarter.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-552AFCE983B2490397CA65025AA6F604"</t>
+  </si>
+  <si>
+    <t>400-69</t>
+  </si>
+  <si>
+    <t>F2LCHK-4-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-41C1C2E05845410E9D8A1A7678AFE45E"</t>
+  </si>
+  <si>
+    <t>400-70</t>
+  </si>
+  <si>
+    <t>F2LCHK-3-A</t>
+  </si>
+  <si>
+    <t>You did not provide OperatingLevelCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-6304A9493A2A40F29C9293C14D82D674"</t>
+  </si>
+  <si>
+    <t>400-72</t>
+  </si>
+  <si>
+    <t>F2LCHK-2-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-A7455776CE9B4FF587A1032DDC11068F"</t>
+  </si>
+  <si>
+    <t>ORIS 2442 (Four Corners Steam Elec Station) Location 4</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>F43 (CO2)</t>
+  </si>
+  <si>
+    <t>F2LCHK-1-B</t>
+  </si>
+  <si>
+    <t>According to the monitoring system record, the monitoring system in this flow-to-load check was not a flow system.</t>
   </si>
 </sst>
 </file>
@@ -4023,7 +4231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4058,20 +4266,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="96">
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4114,10 +4319,19 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4126,11 +4340,11 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4460,6 +4674,85 @@
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4474,26 +4767,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="83"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80">
   <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
@@ -4513,7 +4826,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
@@ -4533,7 +4846,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
@@ -4552,7 +4865,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
@@ -4572,7 +4885,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
@@ -4891,7 +5204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AB6CEE-1A2D-4EDD-BF79-DABF10AD8F60}">
   <dimension ref="A1:K319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
+    <sheetView topLeftCell="A299" workbookViewId="0">
       <selection activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
@@ -15119,6 +15432,1006 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1178DED-FAC2-4896-ADA7-BAB067290A3E}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="98.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1313</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>1348</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1349</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1350</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>1348</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1353</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1356</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1360</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>1366</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A12ED-21A8-440D-BCEA-B358D4E41F2C}">
   <dimension ref="A1:K44"/>
   <sheetViews>
@@ -15844,7 +17157,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>881</v>
       </c>
@@ -15873,7 +17186,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>887</v>
       </c>
@@ -15902,7 +17215,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>887</v>
       </c>
@@ -15931,7 +17244,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>887</v>
       </c>
@@ -15960,7 +17273,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>893</v>
       </c>
@@ -15989,7 +17302,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>893</v>
       </c>
@@ -16018,7 +17331,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>898</v>
       </c>
@@ -16047,7 +17360,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>898</v>
       </c>
@@ -16076,7 +17389,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>898</v>
       </c>
@@ -16105,7 +17418,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>898</v>
       </c>
@@ -16134,7 +17447,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>906</v>
       </c>
@@ -16163,7 +17476,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>906</v>
       </c>
@@ -16192,7 +17505,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>906</v>
       </c>
@@ -16221,7 +17534,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>906</v>
       </c>
@@ -16250,7 +17563,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>906</v>
       </c>
@@ -16432,7 +17745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -17226,7 +18539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C84253-C1F3-40A8-BCD6-786B60222E9D}">
   <dimension ref="A1:J68"/>
   <sheetViews>
@@ -19237,7 +20550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF247E8-4CEE-4E4C-AA1C-A5F6418303B4}">
   <dimension ref="A1:K581"/>
   <sheetViews>
@@ -37882,7 +39195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB95806-BA08-44E5-BECF-767BC3A79B45}">
   <dimension ref="A1:K91"/>
   <sheetViews>

</xml_diff>

<commit_message>
F2LREF Test Case Run Completed
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BF758-7CAD-4A54-A995-FE6A56C6FB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F05E813-8E85-4D50-A778-A43E4C5615D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="APPE" sheetId="6" r:id="rId1"/>
     <sheet name="F2LCHK" sheetId="7" r:id="rId2"/>
-    <sheet name="FF2LBAS" sheetId="4" r:id="rId3"/>
-    <sheet name="FF2LTST" sheetId="3" r:id="rId4"/>
-    <sheet name="LINE" sheetId="1" r:id="rId5"/>
-    <sheet name="RATA" sheetId="2" r:id="rId6"/>
-    <sheet name="UNITDEF" sheetId="5" r:id="rId7"/>
+    <sheet name="F2LREF" sheetId="8" r:id="rId3"/>
+    <sheet name="FF2LBAS" sheetId="4" r:id="rId4"/>
+    <sheet name="FF2LTST" sheetId="3" r:id="rId5"/>
+    <sheet name="LINE" sheetId="1" r:id="rId6"/>
+    <sheet name="RATA" sheetId="2" r:id="rId7"/>
+    <sheet name="UNITDEF" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10315" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10569" uniqueCount="1419">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -4147,13 +4148,169 @@
   </si>
   <si>
     <t>According to the monitoring system record, the monitoring system in this flow-to-load check was not a flow system.</t>
+  </si>
+  <si>
+    <t>F2LREF</t>
+  </si>
+  <si>
+    <t>400-32</t>
+  </si>
+  <si>
+    <t>F2LREF-2-D</t>
+  </si>
+  <si>
+    <t>Another Certification Test record with this test number has already been submitted for this location.  If this is a different test, you must assign it a unique test number.   If you wish to edit the existing test, you should import or download the test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-2FB566F1BACA4A188DD3791B0DD165DA"</t>
+  </si>
+  <si>
+    <t>F2LREF-13-A</t>
+  </si>
+  <si>
+    <t>You defined an invalid ReferenceGrossHeatRate for this test.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>400-36</t>
+  </si>
+  <si>
+    <t>F2LREF-11-A</t>
+  </si>
+  <si>
+    <t>You did not provide AverageGrossUnitLoad, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-51802DAB23C54B86A90276CF664A2225"</t>
+  </si>
+  <si>
+    <t>F2LREF-2-C</t>
+  </si>
+  <si>
+    <t>400-38</t>
+  </si>
+  <si>
+    <t>F2LREF-12-A</t>
+  </si>
+  <si>
+    <t>You defined an invalid ReferenceFlowLoadRatio for this test.  This value must be greater than zero and less than 20,000.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-B92A6FE61C614E31B40ACCF8C75FA092"</t>
+  </si>
+  <si>
+    <t>F2LREF-8-B</t>
+  </si>
+  <si>
+    <t>The reference RATA was performed at different time from the end time reported in the flow-to-load reference data.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-4E5BF3CD209C475ABDE479609ED7D73C"</t>
+  </si>
+  <si>
+    <t>400-45</t>
+  </si>
+  <si>
+    <t>F2LREF-10-A</t>
+  </si>
+  <si>
+    <t>You did not provide AverageReferenceMethodFlow, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCCANX2FNC-D29F19F75A74438FBAA76B1D8A930364"</t>
+  </si>
+  <si>
+    <t>400-52</t>
+  </si>
+  <si>
+    <t>F2LREF-6-B</t>
+  </si>
+  <si>
+    <t>You reported a value of "1" as the CalcSeparateReferenceIndicator, but this is value is only appropriate for a multiple stack.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-CC8627FD01594CE482B5AD750A1CD844"</t>
+  </si>
+  <si>
+    <t>F2LREF-7-A</t>
+  </si>
+  <si>
+    <t>You reported an AverageHourlyHeatInputRate but did not determine the ReferenceGrossHeatRate value.  The hourly heat input rate is only needed if you use the GHR methodology.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-9C9E8019A3044880AFBBA14EA7BC1E6E"</t>
+  </si>
+  <si>
+    <t>F2LREF-4-D</t>
+  </si>
+  <si>
+    <t>The OperatingLevelCode is not designated as a normal load level in the active MonitorLoad record.  Flow-to-load reference data must be based on the RATA for the normal operating level.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-07ECA534ED4A4B50B94DE487FC072024"</t>
+  </si>
+  <si>
+    <t>400-65</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-DF48DF5F54BF446C9CAD7F05FE295EA8"</t>
+  </si>
+  <si>
+    <t>F2LREF-5-C</t>
+  </si>
+  <si>
+    <t>You reported a ReferenceGrossHeatRate value but did not provide the AverageHourlyHeatInputRate.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-11917B3E59334C99BD7F0ECECA2040EB"</t>
+  </si>
+  <si>
+    <t>400-71</t>
+  </si>
+  <si>
+    <t>F2LREF-3-A</t>
+  </si>
+  <si>
+    <t>You did not provide RATATestNumber, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "MCA2F23LHK-9ADD34F690504B2DB0EF6261EBC28476"</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "CHV-SABER-F0098559523641328B59D538A1354863"</t>
+  </si>
+  <si>
+    <t>F43-Q2-2021-1</t>
+  </si>
+  <si>
+    <t>F2LREF-1-B</t>
+  </si>
+  <si>
+    <t>According to the monitoring system record, the Flow-to-load reference data was not for a flow system.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-D4C88AC0994340F2AB7E9E0DB1EF8FCB" "PC49096-389AF24B880A4839B7D1041D3B973F5E"</t>
+  </si>
+  <si>
+    <t>The RATA for Operating Level L contains fewer than nine RATA run records with a run status of "RUNUSED".  A minimum of nine runs are required for each complete operating level test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3B23A43070D74F53AA2DAD83ABFC190C" "CHV-SABER-88B0B970AC8848CD92FCCA64032108E6"</t>
+  </si>
+  <si>
+    <t>F2LREF-9-A</t>
+  </si>
+  <si>
+    <t>The AverageGrossUnitLoad and AverageReferenceMethodFlow could not be recalculated because of invalid data in the reported reference RATA(s).</t>
+  </si>
+  <si>
+    <t>ADMNOVR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4165,6 +4322,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4231,7 +4394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4272,11 +4435,93 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="109">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4767,139 +5012,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="98"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80">
-  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="12">
+  <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66">
-  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93">
+  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="83"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="82"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79">
+  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
-  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53">
+  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15435,8 +15700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1178DED-FAC2-4896-ADA7-BAB067290A3E}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
@@ -16432,6 +16697,941 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284F8D0C-E6B8-46E4-BE14-B585B6CD2EA0}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="74.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="53" style="5" customWidth="1"/>
+    <col min="11" max="11" width="100.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D2" s="6">
+        <v>42411.477083333331</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D3" s="6">
+        <v>42411.477083333331</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42740.288194444445</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42740.288194444445</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42739.6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1381</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42739.6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43186.368055555555</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1384</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D9" s="6">
+        <v>43186.368055555555</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43185.624305555553</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1387</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43185.624305555553</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43495.42291666667</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D13" s="6">
+        <v>43495.42291666667</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43493.613888888889</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1395</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43493.613888888889</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44015.586805555555</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44015.586805555555</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D18" s="6">
+        <v>44015.35833333333</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D19" s="6">
+        <v>44015.35833333333</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>1403</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D20" s="6">
+        <v>44315.677083333336</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44314.429166666669</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1406</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1407</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D22" s="6">
+        <v>44314.429166666669</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="6">
+        <v>43191.665972222225</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="6">
+        <v>43192.326388888891</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6">
+        <v>43192.326388888891</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D26" s="6">
+        <v>44368.693055555559</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D27" s="6">
+        <v>44368.693055555559</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D28" s="6">
+        <v>44368.693055555559</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A12ED-21A8-440D-BCEA-B358D4E41F2C}">
   <dimension ref="A1:K44"/>
   <sheetViews>
@@ -17745,7 +18945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -18539,7 +19739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C84253-C1F3-40A8-BCD6-786B60222E9D}">
   <dimension ref="A1:J68"/>
   <sheetViews>
@@ -20550,7 +21750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF247E8-4CEE-4E4C-AA1C-A5F6418303B4}">
   <dimension ref="A1:K581"/>
   <sheetViews>
@@ -39195,7 +40395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB95806-BA08-44E5-BECF-767BC3A79B45}">
   <dimension ref="A1:K91"/>
   <sheetViews>

</xml_diff>

<commit_message>
7DAY Test Case Run Completed
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F05E813-8E85-4D50-A778-A43E4C5615D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634895A3-66C5-4B55-A2DC-AEA47FD41396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
-    <sheet name="APPE" sheetId="6" r:id="rId1"/>
-    <sheet name="F2LCHK" sheetId="7" r:id="rId2"/>
-    <sheet name="F2LREF" sheetId="8" r:id="rId3"/>
-    <sheet name="FF2LBAS" sheetId="4" r:id="rId4"/>
-    <sheet name="FF2LTST" sheetId="3" r:id="rId5"/>
-    <sheet name="LINE" sheetId="1" r:id="rId6"/>
-    <sheet name="RATA" sheetId="2" r:id="rId7"/>
-    <sheet name="UNITDEF" sheetId="5" r:id="rId8"/>
+    <sheet name="7DAY" sheetId="9" r:id="rId1"/>
+    <sheet name="APPE" sheetId="6" r:id="rId2"/>
+    <sheet name="F2LCHK" sheetId="7" r:id="rId3"/>
+    <sheet name="F2LREF" sheetId="8" r:id="rId4"/>
+    <sheet name="FF2LBAS" sheetId="4" r:id="rId5"/>
+    <sheet name="FF2LTST" sheetId="3" r:id="rId6"/>
+    <sheet name="LINE" sheetId="1" r:id="rId7"/>
+    <sheet name="RATA" sheetId="2" r:id="rId8"/>
+    <sheet name="UNITDEF" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10569" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11212" uniqueCount="1578">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -4304,6 +4305,483 @@
   </si>
   <si>
     <t>ADMNOVR</t>
+  </si>
+  <si>
+    <t>ORIS 991 (IPL - Eagle Valley Generating Station) Location GT1</t>
+  </si>
+  <si>
+    <t>7DAY</t>
+  </si>
+  <si>
+    <t>C01-1</t>
+  </si>
+  <si>
+    <t>C01 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-5-C</t>
+  </si>
+  <si>
+    <t>QAT "PAULDESKTO-AB29DAB24FE34773AEB328AE656A6517" "PAULDESKTO-F936E680AA2B4D4EB9760065D0EE8A0B"</t>
+  </si>
+  <si>
+    <t>C02-1</t>
+  </si>
+  <si>
+    <t>C02 (DL)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-2-B</t>
+  </si>
+  <si>
+    <t>The ComponentTypeCode in the monitoring plan is DL.  This type of component does not require a calibration test.</t>
+  </si>
+  <si>
+    <t>QAT "PAULDESKTO-AB29DAB24FE34773AEB328AE656A6517" "PAULDESKTO-BD1A439323D8411FA73717C72F1612CA"</t>
+  </si>
+  <si>
+    <t>ORIS 991 (IPL - Eagle Valley Generating Station) Location GT2</t>
+  </si>
+  <si>
+    <t>C21-1</t>
+  </si>
+  <si>
+    <t>C21 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-3-A</t>
+  </si>
+  <si>
+    <t>QAT "PAULDESKTO-BEB3B664F7564ABA9A2FDB391B30F821" "PAULDESKTO-A22AE094DAF94B7E8E77158B2C0E1C9F"</t>
+  </si>
+  <si>
+    <t>C22-1</t>
+  </si>
+  <si>
+    <t>C22 (O2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-4-A</t>
+  </si>
+  <si>
+    <t>The TestResultCode indicates that the test was aborted.  CalibrationInjection records for this test will not be evaluated.  If the test was aborted for a reason not related to monitor performance, you should not report the test.</t>
+  </si>
+  <si>
+    <t>QAT "PAULDESKTO-BEB3B664F7564ABA9A2FDB391B30F821" "PAULDESKTO-F01FF52ED9C1425A99D2FD9B2AADA603"</t>
+  </si>
+  <si>
+    <t>ORIS 50292 (Bethpage Energy Center) Location GT1</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-012-1</t>
+  </si>
+  <si>
+    <t>012 (NOX)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-A72D9F4120CB42959C52B10CCB02CD55" "DT3272ZV1-E60006B9EB9842DAB0CB2EB0EFF4D180"</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-013-3</t>
+  </si>
+  <si>
+    <t>013 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-6-A</t>
+  </si>
+  <si>
+    <t>The zero injection date, hour, and/or minute for Zero Injection Date 5/20/2015 is invalid.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-A72D9F4120CB42959C52B10CCB02CD55" "DT3272ZV1-479038334D6942D18E93B1B8DE3EB822"</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-031-2</t>
+  </si>
+  <si>
+    <t>031 (CO2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-7-B</t>
+  </si>
+  <si>
+    <t>The ZeroInjectionDate was not equal to the UpscaleInjectionDate for Zero Injection Date 5/20/2015.  The zero-level and upscale injections reported in the same record must be performed on the same day.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-A72D9F4120CB42959C52B10CCB02CD55" "DT3272ZV1-087B5F6CF08E441F8A28A0AEE0DEC9EB"</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-032-2</t>
+  </si>
+  <si>
+    <t>032 (CO2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-8-A</t>
+  </si>
+  <si>
+    <t>You did not provide ZeroCalibrationError, which is required for Zero Injection Date 5/20/2015.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-A72D9F4120CB42959C52B10CCB02CD55" "DT3272ZV1-64512A44FDE84E1A99FFA6EF97506A07"</t>
+  </si>
+  <si>
+    <t>ORIS 50292 (Bethpage Energy Center) Location GT2</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-012-3</t>
+  </si>
+  <si>
+    <t>SEVNDAY-9-B</t>
+  </si>
+  <si>
+    <t>The value -1.00 in the field UpscaleCalibrationError for Zero Injection Date 5/20/2015 is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-0A56CEF615BB42BDB87E83EB5275639F"</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-013-4</t>
+  </si>
+  <si>
+    <t>SEVNDAY-10-A</t>
+  </si>
+  <si>
+    <t>You did not provide UpscaleGasLevelCode, which is required for Zero Injection Date 5/20/2015.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-A11FFEFCB3FC4B8D8C6E78744BE2EDE8"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-16-A</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 5/20/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-031-4</t>
+  </si>
+  <si>
+    <t>SEVNDAY-12-A</t>
+  </si>
+  <si>
+    <t>You did not provide UpscaleMeasuredValue, which is required for Zero Injection Date 5/20/2015.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-CCB64E01672D4FFB9AB18045653E659F"</t>
+  </si>
+  <si>
+    <t>7DAY-Q22015-032-4</t>
+  </si>
+  <si>
+    <t>SEVNDAY-13-B</t>
+  </si>
+  <si>
+    <t>The value -1.000 in the field ZeroReferenceValue for Zero Injection Date 5/20/2015 is not within the range of valid values.  This value must be greater than or equal to zero.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-EE45A8D72DA042E1974022017936531B"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-15-A</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 5/20/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>7DAY-Q42015-013-1</t>
+  </si>
+  <si>
+    <t>SEVNDAY-11-A</t>
+  </si>
+  <si>
+    <t>You did not provide ZeroMeasuredValue, which is required for Zero Injection Date 11/9/2015.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-6AB38E772172454B8CB693020277A24F"</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 11/9/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>7DAY-Q42015-032-2</t>
+  </si>
+  <si>
+    <t>SEVNDAY-14-A</t>
+  </si>
+  <si>
+    <t>You did not provide UpscaleReferenceValue, which is required for Zero Injection Date 11/9/2015.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-1AFDBDE589FE42A9AD2FA3D97D9D734A"</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 11/9/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>7DAY-Q42015-213-1</t>
+  </si>
+  <si>
+    <t>213 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-17-F</t>
+  </si>
+  <si>
+    <t>The Zero Calibration Error reported for Zero Injection Date 11/9/2015 is inconsistent with the recalculated calibration error for the gas injection or reference signal.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-9475F6FB507D4E869C3915D3AE9BBD10"</t>
+  </si>
+  <si>
+    <t>7DAY-Q42015-232-2</t>
+  </si>
+  <si>
+    <t>232 (CO2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-18-C</t>
+  </si>
+  <si>
+    <t>You reported a value of "1" as the Upscale APS Indicator for Zero Injection Date 11/9/2015, but you must use the standard performance specification criteria for CO2 and O2 components.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-02B24E1727D2437A93812805D7934CC0" "DT3272ZV1-745C7CD20939495FB5B03FE0958FDCBB"</t>
+  </si>
+  <si>
+    <t>ORIS 50292 (Bethpage Energy Center) Location GT3</t>
+  </si>
+  <si>
+    <t>21Q2-NOXH-7DAY</t>
+  </si>
+  <si>
+    <t>310 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-20-A</t>
+  </si>
+  <si>
+    <t>You reported a Test End Date, Hour, and Minute that is not the same as the Injection Date, Hour, and Minute of the last injection in the 7 day calibration test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-2A4BD8E2E84D48709192EC978C09719D" "LT34SHJM2-8661EEECB30D4E5DA52257264B286AC9"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-21-A</t>
+  </si>
+  <si>
+    <t>The test contains fewer than seven calibration injection records.</t>
+  </si>
+  <si>
+    <t>21Q2-NOXL-7DAY</t>
+  </si>
+  <si>
+    <t>QAT "MDC-2A4BD8E2E84D48709192EC978C09719D" "LT34SHJM2-777BB6450ACB4E4B8D7687BBBD55886A"</t>
+  </si>
+  <si>
+    <t>21Q2-O2-7DAY</t>
+  </si>
+  <si>
+    <t>320 (O2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-22-A</t>
+  </si>
+  <si>
+    <t>You have reported more than one value as the UpscaleGasLevelCode in the calibration injection records.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-2A4BD8E2E84D48709192EC978C09719D" "LT34SHJM2-CCFB53FF9C7043DEA439B887FF9C3523"</t>
+  </si>
+  <si>
+    <t>7DAY-Q12018-105-1</t>
+  </si>
+  <si>
+    <t>105 (O2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-19-A</t>
+  </si>
+  <si>
+    <t>You reported a test Begin Date, Hour, and Minute that is not the same as the Injection Date, Hour, and Minute of the first injection in the 7-day calibration test.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-2A4BD8E2E84D48709192EC978C09719D" "LT34SHJM2-09FEF0F5B2A3445A9DDB26D466F826B4"</t>
+  </si>
+  <si>
+    <t>ORIS 50292 (Bethpage Energy Center) Location GT4</t>
+  </si>
+  <si>
+    <t>7DAY-Q22018-206-1</t>
+  </si>
+  <si>
+    <t>206 (NOX)</t>
+  </si>
+  <si>
+    <t>The Zero Calibration Error reported for Zero Injection Date 5/4/2018 is inconsistent with the recalculated calibration error for the gas injection or reference signal.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-5135A4CCD59347F0B5EA4262E78D79C8" "LT5CGR7H2-7E701C2F48BD40378F7C888E9AE658B6"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-23-A</t>
+  </si>
+  <si>
+    <t>The reference values are not consistent with the calibration gas/signal levels reported.  The reference values of zero-level gas injections or signals must be less than those of upscale gas injections.</t>
+  </si>
+  <si>
+    <t>SEVNDAY-24-A</t>
+  </si>
+  <si>
+    <t>The tag value of at least one Zero level reference signal or calibration gas for this test is 88.0%, which does not meet the performance specifications of 40 CFR Part 75.  The concentration of the zero reference signal or calibration gas must be less than or equal to 20.0% of the span value.  The test is invalid.</t>
+  </si>
+  <si>
+    <t>7DAY-Q32020-207-13</t>
+  </si>
+  <si>
+    <t>207 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-18-F</t>
+  </si>
+  <si>
+    <t>The Upscale Calibration Error reported for Zero Injection Date 6/25/2020 is inconsistent with the recalculated calibration error for the gas injection or reference signal.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-5135A4CCD59347F0B5EA4262E78D79C8" "LT34SHJM2-100F5EEA51E54F47B6811F9CA35E562C"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-27-D</t>
+  </si>
+  <si>
+    <t>You have reported a 7-day calibration test, but the recalculated results indicate a failing test.</t>
+  </si>
+  <si>
+    <t>SEVNDAY-25-E</t>
+  </si>
+  <si>
+    <t>The tag value of at least one High level reference calibration gas for this test is 104.0%, which does not meet the applicable performance specifications.  The concentration of the high reference calibration gas must be between 80.0% and 100.0% of the span value.  The test is invalid.</t>
+  </si>
+  <si>
+    <t>7DAY-Q32020-208-5</t>
+  </si>
+  <si>
+    <t>208 (O2)</t>
+  </si>
+  <si>
+    <t>The ZeroInjectionDate was not equal to the UpscaleInjectionDate for Zero Injection Date 6/25/2020.  The zero-level and upscale injections reported in the same record must be performed on the same day.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-5135A4CCD59347F0B5EA4262E78D79C8" "LT34SHJM2-7B00492C69CF48C98577F3BAF8163768"</t>
+  </si>
+  <si>
+    <t>SEVNDAY-26-A</t>
+  </si>
+  <si>
+    <t>This test contains at least two zero-level calibration gas injections or reference signals that were performed on the same day.</t>
+  </si>
+  <si>
+    <t>ORIS 55382 (Thomas A. Smith Energy Facility) Location CCCT1</t>
+  </si>
+  <si>
+    <t>112 (NOX)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-31-B</t>
+  </si>
+  <si>
+    <t>You reported an OnlineOfflineIndicator for Zero Injection Date 5/16/2021 that indicates that the unit was offline, but 7-day calibration test injections must be performed when the unit is online.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3F03FCD6E1C14103B3D6A1EBA54B84C9" "4B23Z91-HQ-D832656FC58243F9A8A20876FC6E9D88"</t>
+  </si>
+  <si>
+    <t>122 (O2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-33-A</t>
+  </si>
+  <si>
+    <t>You did not provide UpscaleAPSIndicator, which is required for Zero Injection Date 5/16/2021.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3F03FCD6E1C14103B3D6A1EBA54B84C9" "4B23Z91-HQ-FF50BBE9C7164535B303E05BEF729A7E"</t>
+  </si>
+  <si>
+    <t>121 (O2)</t>
+  </si>
+  <si>
+    <t>SEVNDAY-32-A</t>
+  </si>
+  <si>
+    <t>You did not provide ZeroAPSIndicator, which is required for Zero Injection Date 6/12/2019.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-3F03FCD6E1C14103B3D6A1EBA54B84C9" "4B23Z91-HQ-65FEBA4862D14F9C9603775114D428BC"</t>
+  </si>
+  <si>
+    <t>ORIS 55382 (Thomas A. Smith Energy Facility) Location CCCT2</t>
+  </si>
+  <si>
+    <t>212 (NOX)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-8ADB7E2796C84D2BA4847FC023F83907" "4B23Z91-HQ-C65F1D235F8647D0815D62282ABAFA41"</t>
+  </si>
+  <si>
+    <t>222 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-8ADB7E2796C84D2BA4847FC023F83907" "4B23Z91-HQ-283907853EE94C17BCAC80AC4AD8141A"</t>
+  </si>
+  <si>
+    <t>221 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-8ADB7E2796C84D2BA4847FC023F83907" "4B23Z91-HQ-1897C5F2034A4190A8E01D21DB1F5E67"</t>
+  </si>
+  <si>
+    <t>ORIS 55382 (Thomas A. Smith Energy Facility) Location CCCT3</t>
+  </si>
+  <si>
+    <t>321 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-7C8BA01B673F46818B57F43A9480448E" "4B23Z91-HQ-98C9940B282E4DE9851DED584CF5E5B1"</t>
+  </si>
+  <si>
+    <t>312 (NOX)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-7C8BA01B673F46818B57F43A9480448E" "4B23Z91-HQ-35DAB2FE023442CCB33587E7E17D7A9B"</t>
+  </si>
+  <si>
+    <t>322 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-7C8BA01B673F46818B57F43A9480448E" "4B23Z91-HQ-36576A9D530E40BDAD2C3E46DFEABEFF"</t>
+  </si>
+  <si>
+    <t>ORIS 55382 (Thomas A. Smith Energy Facility) Location CCCT4</t>
+  </si>
+  <si>
+    <t>421 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-69BF85C161FD4B6494B0C754FE3AD58E" "4B23Z91-HQ-05751ECB766D4E53A52833C7F44C8463"</t>
+  </si>
+  <si>
+    <t>412 (NOX)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-69BF85C161FD4B6494B0C754FE3AD58E" "4B23Z91-HQ-E080D34722E649AA8BEF697BD11E3C17"</t>
+  </si>
+  <si>
+    <t>422 (O2)</t>
+  </si>
+  <si>
+    <t>QAT "MDC-69BF85C161FD4B6494B0C754FE3AD58E" "4B23Z91-HQ-A2B0B8B4625A4DA390EC103AF60AD155"</t>
   </si>
 </sst>
 </file>
@@ -4445,82 +4923,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="123">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4564,19 +4975,10 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4585,11 +4987,11 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4920,6 +5322,161 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5012,159 +5569,179 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107">
-  <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K73" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="98"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="96"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="26">
-  <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121">
+  <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="114"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="110"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="12">
-  <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107">
+  <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="98"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93">
-  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93">
+  <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="84"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="83"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="82"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="83"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79">
-  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80">
+  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="70"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="70"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
-  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66">
+  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53">
-  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5466,6 +6043,2379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5293276-9F89-4E13-BE1D-F189FF00C103}">
+  <dimension ref="A1:K73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="88.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="105.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43140.34097222222</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D3" s="6">
+        <v>43140.338888888888</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43140.338888888888</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43140.34097222222</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43140.34097222222</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D7" s="6">
+        <v>43140.338888888888</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1438</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43140.338888888888</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1447</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D11" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D12" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1452</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D14" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42154.410416666666</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D18" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D19" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D20" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>1469</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D21" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D22" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D23" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1469</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D24" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D25" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D26" s="6">
+        <v>42150.052083333336</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D27" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>1482</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D28" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D29" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>1484</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D30" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>1487</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D31" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D32" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>1489</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D33" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D34" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D35" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>1497</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D36" s="6">
+        <v>42323.374305555553</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D37" s="6">
+        <v>44325.722916666666</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D38" s="6">
+        <v>44325.722916666666</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>1507</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D39" s="6">
+        <v>44325.722916666666</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D40" s="6">
+        <v>44325.723611111112</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D41" s="6">
+        <v>44325.723611111112</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D42" s="6">
+        <v>44325.722916666666</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>1513</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D43" s="6">
+        <v>44325.722916666666</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D44" s="6">
+        <v>43145.769444444442</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>1518</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D45" s="6">
+        <v>43145.769444444442</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D46" s="6">
+        <v>43269.351388888892</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>1523</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D47" s="6">
+        <v>43269.351388888892</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>1526</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D48" s="6">
+        <v>43269.351388888892</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D49" s="6">
+        <v>43269.351388888892</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D50" s="6">
+        <v>44015.101388888892</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D51" s="6">
+        <v>44015.101388888892</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>1535</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D52" s="6">
+        <v>44015.101388888892</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>1537</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D53" s="6">
+        <v>44015.101388888892</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D54" s="6">
+        <v>44015.099305555559</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>1540</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D55" s="6">
+        <v>44015.099305555559</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>1518</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D56" s="6">
+        <v>44015.099305555559</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D57" s="6">
+        <v>44015.099305555559</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C58" s="1">
+        <v>112</v>
+      </c>
+      <c r="D58" s="6">
+        <v>44338.388194444444</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>1547</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C59" s="1">
+        <v>112</v>
+      </c>
+      <c r="D59" s="6">
+        <v>44338.388194444444</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C60" s="1">
+        <v>112</v>
+      </c>
+      <c r="D60" s="6">
+        <v>44338.388194444444</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C61" s="1">
+        <v>122</v>
+      </c>
+      <c r="D61" s="6">
+        <v>44338.39166666667</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>1551</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C62" s="1">
+        <v>122</v>
+      </c>
+      <c r="D62" s="6">
+        <v>44338.39166666667</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C63" s="1">
+        <v>4</v>
+      </c>
+      <c r="D63" s="6">
+        <v>43634.341666666667</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>1555</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C64" s="1">
+        <v>4</v>
+      </c>
+      <c r="D64" s="6">
+        <v>43634.341666666667</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C65" s="1">
+        <v>212</v>
+      </c>
+      <c r="D65" s="6">
+        <v>44338.430555555555</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C66" s="1">
+        <v>222</v>
+      </c>
+      <c r="D66" s="6">
+        <v>44338.434027777781</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C67" s="1">
+        <v>5</v>
+      </c>
+      <c r="D67" s="6">
+        <v>43649.646527777775</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="6">
+        <v>43625.430555555555</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C69" s="1">
+        <v>312</v>
+      </c>
+      <c r="D69" s="6">
+        <v>44336.47152777778</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C70" s="1">
+        <v>322</v>
+      </c>
+      <c r="D70" s="6">
+        <v>44336.474999999999</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="6">
+        <v>43628.472222222219</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C72" s="1">
+        <v>412</v>
+      </c>
+      <c r="D72" s="6">
+        <v>44333.513194444444</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C73" s="1">
+        <v>422</v>
+      </c>
+      <c r="D73" s="6">
+        <v>44333.51666666667</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AB6CEE-1A2D-4EDD-BF79-DABF10AD8F60}">
   <dimension ref="A1:K319"/>
   <sheetViews>
@@ -15696,7 +18646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1178DED-FAC2-4896-ADA7-BAB067290A3E}">
   <dimension ref="A1:K33"/>
   <sheetViews>
@@ -16696,11 +19646,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284F8D0C-E6B8-46E4-BE14-B585B6CD2EA0}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -17631,7 +20581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A12ED-21A8-440D-BCEA-B358D4E41F2C}">
   <dimension ref="A1:K44"/>
   <sheetViews>
@@ -18945,7 +21895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -19739,7 +22689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C84253-C1F3-40A8-BCD6-786B60222E9D}">
   <dimension ref="A1:J68"/>
   <sheetViews>
@@ -21750,7 +24700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF247E8-4CEE-4E4C-AA1C-A5F6418303B4}">
   <dimension ref="A1:K581"/>
   <sheetViews>
@@ -40395,7 +43345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB95806-BA08-44E5-BECF-767BC3A79B45}">
   <dimension ref="A1:K91"/>
   <sheetViews>

</xml_diff>

<commit_message>
General Test Check Type Testcases
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0E3EA8-7EBF-43F4-A199-A00652BB42FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C339F76-1B1D-4C82-92BB-9D42DA5EC0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="7DAY" sheetId="9" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="ONOFF" sheetId="10" r:id="rId11"/>
     <sheet name="RATA" sheetId="2" r:id="rId12"/>
     <sheet name="UNITDEF" sheetId="5" r:id="rId13"/>
+    <sheet name="TEST Check Type" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12832" uniqueCount="1919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13422" uniqueCount="1990">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -5809,13 +5810,229 @@
   </si>
   <si>
     <t>A transmitter transducer test with this test number has been previously submitted. You must assign a different test number.</t>
+  </si>
+  <si>
+    <t>201501250645CO2</t>
+  </si>
+  <si>
+    <t>TEST-8-A</t>
+  </si>
+  <si>
+    <t>You did not provide SpanScaleCode, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-9987DDF633104765B9AA755E1EA15E90"</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/25/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/26/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/27/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/28/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/29/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/30/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Zero injection calculations reported for Zero Injection Date 1/31/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/27/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/31/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/30/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/29/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/28/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/25/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>The software could not evaluate the Upscale injection calculations reported for Zero Injection Date 1/26/2015, because of the errors listed above.</t>
+  </si>
+  <si>
+    <t>NAX (NOX)</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "CHV-LGIANN-30584F105CE4476CB35F1E1BC7DF280E"</t>
+  </si>
+  <si>
+    <t>TEST-9-C</t>
+  </si>
+  <si>
+    <t>The tested component is not part of any monitoring system.</t>
+  </si>
+  <si>
+    <t>20210713113539NOX</t>
+  </si>
+  <si>
+    <t>TEST-1-A</t>
+  </si>
+  <si>
+    <t>You did not provide BeginDate, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-C42757B58FA54F92A3A178BB053C2E78"</t>
+  </si>
+  <si>
+    <t>20210713113539SO2</t>
+  </si>
+  <si>
+    <t>TEST-2-B</t>
+  </si>
+  <si>
+    <t>The value 24 in the field BeginHour for this test is not within the range of valid values from 0 to 23.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-3C64FBE60DAA4767B39FF0C0F24A0E4A"</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-BB24791354734E67B2CBA5BC85A46F12"</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-EBBFBA13973A41A69A9DDD246386BD10"</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-F87E825735454405A0FD60065958452D"</t>
+  </si>
+  <si>
+    <t>FLO (FLOW)</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-F90C099FDA694744AF3C24D64E2A5DE3"</t>
+  </si>
+  <si>
+    <t>TEST-3-C</t>
+  </si>
+  <si>
+    <t>The value 61 in the field BeginMinute for this test is not within the range of valid values from 0 to 59.</t>
+  </si>
+  <si>
+    <t>TEST-5-B</t>
+  </si>
+  <si>
+    <t>The value 24 in the field EndHour for this test is not within the range of valid values from 0 to 23.</t>
+  </si>
+  <si>
+    <t>TEST-6-C</t>
+  </si>
+  <si>
+    <t>The value 61 in the field EndMinute for this test is not within the range of valid values from 0 to 59.</t>
+  </si>
+  <si>
+    <t>LEAK</t>
+  </si>
+  <si>
+    <t>TEST-16-D</t>
+  </si>
+  <si>
+    <t>The SampleAcquisitionMethodCode of the component associated with this test is invalid.  Leak checks are only performed on differential pressure (DP) flow monitors.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-488E42008B434177BC7D7BFF138D18EF" "CHV-LGIANN-5CA82B0AA75C42BA832B406B17D752CC"</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>FL1 (FLOW)</t>
+  </si>
+  <si>
+    <t>TEST-17-C</t>
+  </si>
+  <si>
+    <t>You reported the value INITIAL, which is not in the list of valid values for this test type, in the field TestReasonCode for this test.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-488E42008B434177BC7D7BFF138D18EF" "CHV-LGIANN-C80ACCC82C0D4F6FB097F190E213831F"</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>XX4 (DAHS)</t>
+  </si>
+  <si>
+    <t>TEST-14-A</t>
+  </si>
+  <si>
+    <t>You did not provide TestDescription, which is required for this test.</t>
+  </si>
+  <si>
+    <t>QAT "TWCORNEL5-488E42008B434177BC7D7BFF138D18EF" "CHV-LGIANN-5A41B20E87C54C42B987817CF8101A5C"</t>
+  </si>
+  <si>
+    <t>TEST-15-A</t>
+  </si>
+  <si>
+    <t>The GracePeriodIndicator is not appropriate for this test type.</t>
+  </si>
+  <si>
+    <t>TEST-23-D</t>
+  </si>
+  <si>
+    <t>An injection protocol is not required for this test type.</t>
+  </si>
+  <si>
+    <t>ORIS 56476 (Gateway Generating Station) Location GT1</t>
+  </si>
+  <si>
+    <t>GT1-VT001</t>
+  </si>
+  <si>
+    <t>004 (GFFM)</t>
+  </si>
+  <si>
+    <t>TEST-18-A</t>
+  </si>
+  <si>
+    <t>QAT "MDC-985E2491326D4848BB4E753FA4AA301E" "LTGO295726-75DCE01EB6B94A32A7FAE2C1CBD9E552"</t>
+  </si>
+  <si>
+    <t>TEST-20-C</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>TEST-22-A</t>
+  </si>
+  <si>
+    <t>A Monitoring Plan associated with this test has critical errors.  You must correct all active and future Monitoring Plans containing the location in this test in order to submit this test to be loaded on EPA's host system.</t>
+  </si>
+  <si>
+    <t>MP Severity Code source view CAMDECMPSWKS VW_MONITOR_PLAN_LOCATION grabs CHECK_SESSION SEVERITY_CODE from the CAMDECMPSAUX schema instead of the CAMDECMPSWKS schema.</t>
+  </si>
+  <si>
+    <t>Failed executing method 'ThrowInvalidOperationException_InvalidOperation_NoValue'.
+Nullable object must have a value.
+   at System.Nullable`1.get_Value()_x000D_
+   at ECMPS.Checks.TestChecks.cPgvpChecks.PGVP4(cCategory category, Boolean&amp; log) in C:\Dev\CAMDDevelopment\easey-quartz-scheduler\CheckEngine\QA\Checks\PgvpChecks.cs:line 319</t>
+  </si>
+  <si>
+    <t>PGVP-4 attempts to convert the BEGIN_DATE but does not expect the date to be null and throws an exception.  The testcase is for TEST-1-A, which fires if the date is null.  This exception occurs for both ECMPS 1.0 and 2.0.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5833,6 +6050,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5899,7 +6123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5946,89 +6170,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="179">
+  <dxfs count="193">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6084,19 +6244,10 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6380,6 +6531,164 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6911,259 +7220,279 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
   <autoFilter ref="A1:K73" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="167"/>
-    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="166"/>
-    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="165"/>
+    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="186"/>
+    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="183"/>
+    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="182"/>
+    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="181"/>
+    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="180"/>
+    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="76"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
   <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="57"/>
-    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K65" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="164" dataDxfId="162" headerRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="160"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="159"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="158"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="157"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="156"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="155"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="154"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="153"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="152"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="151"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="174"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="173"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="172"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="171"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="170"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="168"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="167"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="166"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="150" dataDxfId="148" headerRowBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="164" dataDxfId="162" headerRowBorderDxfId="163">
   <autoFilter ref="A1:K43" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="145"/>
-    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="144"/>
-    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="143"/>
-    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="142"/>
-    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="141"/>
-    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="140"/>
-    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="139"/>
-    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="138"/>
-    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="137"/>
+    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="160"/>
+    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="158"/>
+    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="157"/>
+    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="156"/>
+    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="155"/>
+    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="154"/>
+    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="153"/>
+    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="152"/>
+    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="136" dataDxfId="134" headerRowBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="150" dataDxfId="148" headerRowBorderDxfId="149">
   <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="132"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="130"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="129"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="128"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="127"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="126"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="125"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="124"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="144"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="143"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="142"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="141"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="140"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="139"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="138"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="137"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="122" headerRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="136" headerRowBorderDxfId="135">
   <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="126"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
   <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
   <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="83"/>
+    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80">
   <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="70"/>
+    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35795,6 +36124,2140 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D196CC-3DC9-4A6C-BAF4-BA1549D5FF19}">
+  <dimension ref="A1:K65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="75.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="104.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D2" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1920</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1921</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D3" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1923</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>1924</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1925</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1926</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1927</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1928</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1929</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D11" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1930</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D12" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1931</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>1932</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D14" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1933</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1934</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1935</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42035.284722222219</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>1936</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="6">
+        <v>42035</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1937</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1507</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="6">
+        <v>42035</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1937</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1939</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>1940</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="6">
+        <v>42035</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1937</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1988</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>1989</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D22" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1942</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>1943</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D24" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D25" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1946</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1947</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D26" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D27" s="6">
+        <v>44390.533333333333</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="6">
+        <v>44410.140277777777</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="6">
+        <v>44410.140277777777</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="6">
+        <v>44410.667361111111</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>1954</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>1955</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="6">
+        <v>44410.667361111111</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="6">
+        <v>44410.667361111111</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="6">
+        <v>44410.667361111111</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="1">
+        <v>44411.000694444447</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>1956</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>1957</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="1">
+        <v>44411.000694444447</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="1">
+        <v>44411.000694444447</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44411.000694444447</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" s="1">
+        <v>44410.709027777775</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>1958</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>1959</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" s="1">
+        <v>44410.709027777775</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" s="1">
+        <v>44410.709027777775</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D50" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>1986</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D54" s="6">
+        <v>44379.611805555556</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1961</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>1962</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="D57" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>1965</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>1966</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>1967</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="D58" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>1965</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>1961</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>1962</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C59" s="3">
+        <v>123</v>
+      </c>
+      <c r="D59" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>1972</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C60" s="3">
+        <v>123</v>
+      </c>
+      <c r="D60" s="6">
+        <v>44552</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>1975</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D61" s="6">
+        <v>44250.609722222223</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>1977</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" s="6">
+        <v>44250.609722222223</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" s="6">
+        <v>44250.609722222223</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D64" s="6">
+        <v>39843.708333333336</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D65" s="6">
+        <v>39843.708333333336</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AB6CEE-1A2D-4EDD-BF79-DABF10AD8F60}">
   <dimension ref="A1:K319"/>
@@ -51475,7 +53938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F251FFA4-DA4E-420C-9FBD-B96432E43209}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -52269,7 +54732,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1202</v>
       </c>
@@ -52301,7 +54764,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1202</v>
       </c>

</xml_diff>

<commit_message>
PGVP Check Type Testcases
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C339F76-1B1D-4C82-92BB-9D42DA5EC0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23707B10-5E85-4B74-96C7-EC9B310FBED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="7DAY" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="ONOFF" sheetId="10" r:id="rId11"/>
     <sheet name="RATA" sheetId="2" r:id="rId12"/>
     <sheet name="UNITDEF" sheetId="5" r:id="rId13"/>
-    <sheet name="TEST Check Type" sheetId="14" r:id="rId14"/>
+    <sheet name="Check Type PGVP" sheetId="15" r:id="rId14"/>
+    <sheet name="Check Type TEST" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13422" uniqueCount="1990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13658" uniqueCount="2018">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -6026,6 +6027,90 @@
   </si>
   <si>
     <t>PGVP-4 attempts to convert the BEGIN_DATE but does not expect the date to be null and throws an exception.  The testcase is for TEST-1-A, which fires if the date is null.  This exception occurs for both ECMPS 1.0 and 2.0.</t>
+  </si>
+  <si>
+    <t>20210419084622CD1</t>
+  </si>
+  <si>
+    <t>PGVP-11-A</t>
+  </si>
+  <si>
+    <t>You reported an GasTypeCode that is not appropriate for the component type or the test reference method for Gas Level HIGH Gas Type AIR.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-BE6DED44FBE145D6B3CF0E9BB40CAD46"</t>
+  </si>
+  <si>
+    <t>20210419084622NX1</t>
+  </si>
+  <si>
+    <t>PGVP-10-D</t>
+  </si>
+  <si>
+    <t>You reported a GasTypeCode of "ZERO" which is only appropriate for the low level calibration of a reference analyzer used in Reference Method 3A, 6C, or 7E testing.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-8B094C53547D424EB92D4420A44EACBC"</t>
+  </si>
+  <si>
+    <t>20211012083705CD1</t>
+  </si>
+  <si>
+    <t>PGVP-2-A</t>
+  </si>
+  <si>
+    <t>You did not provide CylinderIdentifier, which is required for Gas Level HIGH Gas Type CO2,NO,NOX,BALN.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-26BCE00CFDDD4545ACF6CBCEC7399200"</t>
+  </si>
+  <si>
+    <t>20211012083705NX1</t>
+  </si>
+  <si>
+    <t>PGVP-3-B</t>
+  </si>
+  <si>
+    <t>You reported the value B220191, which is not in the list of valid values, in the field VendorIdentifier for Cylinder Identifier CC44728.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-7EBFA586EAB2493F92FF0341E03CDC14"</t>
+  </si>
+  <si>
+    <t>20211012091507CD1</t>
+  </si>
+  <si>
+    <t>You reported an ExpirationDate for the cylinder that is prior to the date of the test for Cylinder Identifier CC44728.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-48F8FBBDDF5142339034084C2FFCF856"</t>
+  </si>
+  <si>
+    <t>20211012091507NX1</t>
+  </si>
+  <si>
+    <t>PGVP-5-C</t>
+  </si>
+  <si>
+    <t>You reported an GasLevelCode of "AIR" for Gas Level MID Gas Type AIR, which indicates the use of purified air material, but this material can only be used for a high-level calibration.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-A99B4D9EDB914CCBB5F75F738C9F6F5C"</t>
+  </si>
+  <si>
+    <t>PGVP-11-C</t>
+  </si>
+  <si>
+    <t>You reported an GasTypeCode that is not appropriate for the component type or the test reference method for Gas Level MID Gas Type AIR.</t>
+  </si>
+  <si>
+    <t>You incorrectly reported a Protocol Gas Record for Cylinder Identifier CC357282.  You should only report a Protocol Gas record for a RATA performed using instrumental reference methods 3A, 6C, or 7E.</t>
+  </si>
+  <si>
+    <t>You incorrectly reported a Protocol Gas Record for Cylinder Identifier CC419382.  You should only report a Protocol Gas record for a RATA performed using instrumental reference methods 3A, 6C, or 7E.</t>
+  </si>
+  <si>
+    <t>You incorrectly reported a Protocol Gas Record for Cylinder Identifier CC360515.  You should only report a Protocol Gas record for a RATA performed using instrumental reference methods 3A, 6C, or 7E.</t>
   </si>
 </sst>
 </file>
@@ -6180,7 +6265,86 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="193">
+  <dxfs count="207">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -7220,279 +7384,299 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="206" dataDxfId="204" headerRowBorderDxfId="205">
   <autoFilter ref="A1:K73" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="188"/>
-    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="185"/>
-    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="184"/>
-    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="183"/>
-    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="182"/>
-    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="181"/>
-    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="180"/>
-    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="203"/>
+    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="202"/>
+    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="201"/>
+    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="198"/>
+    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="197"/>
+    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="196"/>
+    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="195"/>
+    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="194"/>
+    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="63"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="76"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
   <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K26" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{141A1F22-04AC-41C4-A9F5-CA2D856537D2}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{682EB442-4EFC-4943-86B4-811065481E58}" name="Test Type" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A5BCB04C-743D-46FA-B0DB-84CF0B6BBC8E}" name="Test Number" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{337B62FF-2ACC-49AF-ACCD-33722D3A358A}" name="Test Date-Time" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{CA9A9114-48D7-4C09-9D29-E09FD186CBA4}" name="Sys/Comp Info" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{19FB15F6-B8AD-4984-9641-8937F6CFB220}" name="Severity" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B429ED75-C4D0-4170-8D54-B8270FFB8774}" name="EASEY Result Code" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{B11B957A-B097-47B2-A383-93BC12EF8B7D}" name="Fired" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{C1D59F6D-98B3-4861-AE30-E527BF23B4D6}" name="EASEY Result" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{AF930BC6-6880-489A-BB78-667B6B0662F2}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{BDA74063-BCCA-4147-84D8-3ACA73246EC1}" name="Command Line Parameters" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="27">
   <autoFilter ref="A1:K65" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="167"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="166"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="165"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="186"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="183"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="182"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="181"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="180"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="164" dataDxfId="162" headerRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
   <autoFilter ref="A1:K43" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="160"/>
-    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="159"/>
-    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="158"/>
-    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="157"/>
-    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="156"/>
-    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="155"/>
-    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="154"/>
-    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="153"/>
-    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="152"/>
-    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="151"/>
+    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="174"/>
+    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="173"/>
+    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="172"/>
+    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="171"/>
+    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="170"/>
+    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="168"/>
+    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="167"/>
+    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="166"/>
+    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="150" dataDxfId="148" headerRowBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="164" dataDxfId="162" headerRowBorderDxfId="163">
   <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="145"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="144"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="143"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="142"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="141"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="140"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="139"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="138"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="137"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="160"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="158"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="157"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="156"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="155"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="154"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="153"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="152"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="136" headerRowBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="150" headerRowBorderDxfId="149">
   <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="128"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="127"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="126"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="125"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
   <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="126"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
   <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
   <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="83"/>
+    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -36125,11 +36309,881 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307E8187-44DF-4FB9-8580-48A85C7DC54A}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="112.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="39.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="96.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44305.404166666667</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1991</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1992</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44305.404166666667</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D4" s="6">
+        <v>44305.404166666667</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1996</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44305.404166666667</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D6" s="6">
+        <v>44481.382638888892</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>2000</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44481.382638888892</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D8" s="6">
+        <v>44481.382638888892</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2003</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>2004</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D9" s="6">
+        <v>44481.382638888892</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D10" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2010</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>2011</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D14" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2013</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>2014</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44481.410416666666</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>2015</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>2016</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D22" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>2017</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D196CC-3DC9-4A6C-BAF4-BA1549D5FF19}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
AETB Check Type Testcases
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23707B10-5E85-4B74-96C7-EC9B310FBED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE29CC-5574-4418-99D7-C45142C1B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="809" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="7DAY" sheetId="9" r:id="rId1"/>
@@ -26,8 +26,9 @@
     <sheet name="ONOFF" sheetId="10" r:id="rId11"/>
     <sheet name="RATA" sheetId="2" r:id="rId12"/>
     <sheet name="UNITDEF" sheetId="5" r:id="rId13"/>
-    <sheet name="Check Type PGVP" sheetId="15" r:id="rId14"/>
-    <sheet name="Check Type TEST" sheetId="14" r:id="rId15"/>
+    <sheet name="Check Type AETB" sheetId="16" r:id="rId14"/>
+    <sheet name="Check Type PGVP" sheetId="15" r:id="rId15"/>
+    <sheet name="Check Type TEST" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13658" uniqueCount="2018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13948" uniqueCount="2054">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -6111,6 +6112,114 @@
   </si>
   <si>
     <t>You incorrectly reported a Protocol Gas Record for Cylinder Identifier CC360515.  You should only report a Protocol Gas record for a RATA performed using instrumental reference methods 3A, 6C, or 7E.</t>
+  </si>
+  <si>
+    <t>AETB-9-C</t>
+  </si>
+  <si>
+    <t>You reported an ExamDate that is more than five years prior to the date of the test for Benjamin A. Chalk.  AETB exams expire in five years.</t>
+  </si>
+  <si>
+    <t>AETB-4-A</t>
+  </si>
+  <si>
+    <t>You did not provide AETBName, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-5-A</t>
+  </si>
+  <si>
+    <t>You did not provide AETBPhoneNumber, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-6-A</t>
+  </si>
+  <si>
+    <t>You did not provide AETBEmail, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-7-A</t>
+  </si>
+  <si>
+    <t>You did not provide ProviderName, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-8-A</t>
+  </si>
+  <si>
+    <t>You did not provide ProviderEmail, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-9-A</t>
+  </si>
+  <si>
+    <t>You did not provide ExamDate, which is required for a A. a.</t>
+  </si>
+  <si>
+    <t>AETB-10-B</t>
+  </si>
+  <si>
+    <t>Air Emissions Testing Records are not required for Hg, HCl, HF, or ST tests.</t>
+  </si>
+  <si>
+    <t>201602150844MA3</t>
+  </si>
+  <si>
+    <t>You did not provide AETBEmail, which is required for Benjamin A. Chalk.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-DAB99C69B32643149B6489A1159629B8"</t>
+  </si>
+  <si>
+    <t>201703281312MA3</t>
+  </si>
+  <si>
+    <t>AETB-2-B</t>
+  </si>
+  <si>
+    <t>The value 2 in the QIFirstName for 2 M. Rew does not have the expected format.  Please confirm that this value is reported correctly.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-40EE1436487A491386C9DEF9D97BF0C9"</t>
+  </si>
+  <si>
+    <t>201802270921MA3</t>
+  </si>
+  <si>
+    <t>You did not provide ProviderName, which is required for Judd M. Rew.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-22F251FBE908456FA602381683DB2F70"</t>
+  </si>
+  <si>
+    <t>201901220932MA3</t>
+  </si>
+  <si>
+    <t>AETB-3-A</t>
+  </si>
+  <si>
+    <t>The value 3 in the QIMiddleInitial for Judd 3. Rew does not have the expected format.  Please confirm that this value is reported correctly.</t>
+  </si>
+  <si>
+    <t>QAT "MDC-68FF9CD5F0C2464E85FD2A3C15D5A670" "TWCORNEL5-6CAA42CFC0EE44A3BFC1878FE0EA59EF"</t>
+  </si>
+  <si>
+    <t>AETB-5-B</t>
+  </si>
+  <si>
+    <t>The value 2513317560 in the AETBPhoneNumber for Judd M. Rew does not have the expected format.  Please confirm that this value is reported correctly.</t>
+  </si>
+  <si>
+    <t>You did not provide AETBName, which is required for Judd M. Rew.</t>
+  </si>
+  <si>
+    <t>AETB-1-B</t>
+  </si>
+  <si>
+    <t>The value 1 in the QILastName for Judd M. 1 does not have the expected format.  Please confirm that this value is reported correctly.</t>
+  </si>
+  <si>
+    <t>You did not provide ProviderEmail, which is required for Judd M. Rew.</t>
   </si>
 </sst>
 </file>
@@ -6265,16 +6374,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="207">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="221">
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -6323,7 +6423,13 @@
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6331,6 +6437,53 @@
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6344,27 +6497,6 @@
           <color theme="0"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6408,6 +6540,18 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6418,10 +6562,54 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -7384,299 +7572,319 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="206" dataDxfId="204" headerRowBorderDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="220" dataDxfId="218" headerRowBorderDxfId="219">
   <autoFilter ref="A1:K73" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="203"/>
-    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="202"/>
-    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="201"/>
-    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="200"/>
-    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="199"/>
-    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="198"/>
-    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="197"/>
-    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="196"/>
-    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="195"/>
-    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="194"/>
-    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="193"/>
+    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="217"/>
+    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="216"/>
+    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="215"/>
+    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="214"/>
+    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="213"/>
+    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="212"/>
+    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="211"/>
+    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="209"/>
+    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="208"/>
+    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="207"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="76"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="85"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82">
   <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="57"/>
-    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
-  <autoFilter ref="A1:K26" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K32" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{141A1F22-04AC-41C4-A9F5-CA2D856537D2}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{682EB442-4EFC-4943-86B4-811065481E58}" name="Test Type" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{A5BCB04C-743D-46FA-B0DB-84CF0B6BBC8E}" name="Test Number" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{337B62FF-2ACC-49AF-ACCD-33722D3A358A}" name="Test Date-Time" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{CA9A9114-48D7-4C09-9D29-E09FD186CBA4}" name="Sys/Comp Info" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{19FB15F6-B8AD-4984-9641-8937F6CFB220}" name="Severity" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B429ED75-C4D0-4170-8D54-B8270FFB8774}" name="EASEY Result Code" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{B11B957A-B097-47B2-A383-93BC12EF8B7D}" name="Fired" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{C1D59F6D-98B3-4861-AE30-E527BF23B4D6}" name="EASEY Result" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{AF930BC6-6880-489A-BB78-667B6B0662F2}" name="Notes" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{BDA74063-BCCA-4147-84D8-3ACA73246EC1}" name="Command Line Parameters" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{CEF40D72-5DCC-4B34-AFF0-DB646EE7F1D9}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{73E21D38-0138-4A9D-92D7-F5A45463FD70}" name="Test Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F42AD8C2-F06C-4997-B9FA-A329126E0DFF}" name="Test Number" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{854FA5EA-A370-4202-BA3A-9FA3AB721241}" name="Test Date-Time" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7732B98C-AAD5-4156-A763-0BC4DE759B93}" name="Sys/Comp Info" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{45B5508A-A4AD-4CFF-B677-AD9882050109}" name="Severity" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{C256B736-EB39-4718-8D5D-E6109D13DA65}" name="EASEY Result Code" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{924700DB-01C4-4CC8-9378-33C861B04674}" name="Fired" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{443A7749-F8EE-4346-8DAB-AB037E910CC8}" name="EASEY Result" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{17370406-1790-475D-A379-C70F7A67E837}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{52FD404F-F0C8-42CF-85B7-842E44A87945}" name="Command Line Parameters" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+  <autoFilter ref="A1:K26" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{141A1F22-04AC-41C4-A9F5-CA2D856537D2}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{682EB442-4EFC-4943-86B4-811065481E58}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{A5BCB04C-743D-46FA-B0DB-84CF0B6BBC8E}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{337B62FF-2ACC-49AF-ACCD-33722D3A358A}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{CA9A9114-48D7-4C09-9D29-E09FD186CBA4}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{19FB15F6-B8AD-4984-9641-8937F6CFB220}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{B429ED75-C4D0-4170-8D54-B8270FFB8774}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{B11B957A-B097-47B2-A383-93BC12EF8B7D}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{C1D59F6D-98B3-4861-AE30-E527BF23B4D6}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{AF930BC6-6880-489A-BB78-667B6B0662F2}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{BDA74063-BCCA-4147-84D8-3ACA73246EC1}" name="Command Line Parameters" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K65" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="206" dataDxfId="204" headerRowBorderDxfId="205">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="188"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="185"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="184"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="183"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="182"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="181"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="180"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="203"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="202"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="201"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="198"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="197"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="196"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="195"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="194"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
   <autoFilter ref="A1:K43" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="167"/>
-    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="166"/>
-    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="165"/>
+    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="186"/>
+    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="183"/>
+    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="182"/>
+    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="181"/>
+    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="180"/>
+    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="164" dataDxfId="162" headerRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
   <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="160"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="159"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="158"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="157"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="156"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="155"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="154"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="153"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="152"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="151"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="174"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="173"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="172"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="171"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="170"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="168"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="167"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="166"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="150" headerRowBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="164" headerRowBorderDxfId="163">
   <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="156"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="155"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="154"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="153"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150">
   <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="128"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="127"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="126"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="125"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="126"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
   <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
   <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="84"/>
-    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -36309,10 +36517,1072 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85F61AB-9DA3-44EF-9664-ED9383A7DC6E}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="115.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="102.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43920.578472222223</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2018</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>2019</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="6">
+        <v>43920.578472222223</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43920.578472222223</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>2021</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2022</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>2023</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>2025</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2026</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>2027</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>2029</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2030</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>2031</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2032</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>2033</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43920.741666666669</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42415.574305555558</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>2035</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D14" s="6">
+        <v>42415.574305555558</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42822.741666666669</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2038</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>2039</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42822.741666666669</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43158.572916666664</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>2026</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>2042</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43158.572916666664</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43158.572916666664</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D20" s="6">
+        <v>43158.572916666664</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D21" s="6">
+        <v>43487.588888888888</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>2045</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>2046</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D22" s="6">
+        <v>43487.588888888888</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D23" s="6">
+        <v>43600.525694444441</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>2048</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D24" s="6">
+        <v>43600.525694444441</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D25" s="6">
+        <v>43600.525694444441</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>2050</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D28" s="6">
+        <v>43837.533333333333</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D29" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2051</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>2052</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44257.670138888891</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D31" s="6">
+        <v>44264.519444444442</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D32" s="6">
+        <v>44264.519444444442</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307E8187-44DF-4FB9-8580-48A85C7DC54A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -37178,7 +38448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D196CC-3DC9-4A6C-BAF4-BA1549D5FF19}">
   <dimension ref="A1:K65"/>
   <sheetViews>

</xml_diff>

<commit_message>
QCE Testcases with some TEE.
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE29CC-5574-4418-99D7-C45142C1B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60D5ECC-BD9B-46FB-BD40-5D7AF9FA7D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="809" activeTab="13" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="809" activeTab="3" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="7DAY" sheetId="9" r:id="rId1"/>
     <sheet name="APPE" sheetId="6" r:id="rId2"/>
     <sheet name="CYCLE" sheetId="11" r:id="rId3"/>
-    <sheet name="F2LCHK" sheetId="7" r:id="rId4"/>
-    <sheet name="F2LREF" sheetId="8" r:id="rId5"/>
-    <sheet name="FF2LBAS" sheetId="4" r:id="rId6"/>
-    <sheet name="FF2LTST" sheetId="3" r:id="rId7"/>
-    <sheet name="FFACC" sheetId="13" r:id="rId8"/>
-    <sheet name="FFACCTT" sheetId="12" r:id="rId9"/>
-    <sheet name="LINE" sheetId="1" r:id="rId10"/>
-    <sheet name="ONOFF" sheetId="10" r:id="rId11"/>
-    <sheet name="RATA" sheetId="2" r:id="rId12"/>
-    <sheet name="UNITDEF" sheetId="5" r:id="rId13"/>
-    <sheet name="Check Type AETB" sheetId="16" r:id="rId14"/>
-    <sheet name="Check Type PGVP" sheetId="15" r:id="rId15"/>
-    <sheet name="Check Type TEST" sheetId="14" r:id="rId16"/>
+    <sheet name="EVENT" sheetId="17" r:id="rId4"/>
+    <sheet name="F2LCHK" sheetId="7" r:id="rId5"/>
+    <sheet name="F2LREF" sheetId="8" r:id="rId6"/>
+    <sheet name="FF2LBAS" sheetId="4" r:id="rId7"/>
+    <sheet name="FF2LTST" sheetId="3" r:id="rId8"/>
+    <sheet name="FFACC" sheetId="13" r:id="rId9"/>
+    <sheet name="FFACCTT" sheetId="12" r:id="rId10"/>
+    <sheet name="LINE" sheetId="1" r:id="rId11"/>
+    <sheet name="ONOFF" sheetId="10" r:id="rId12"/>
+    <sheet name="RATA" sheetId="2" r:id="rId13"/>
+    <sheet name="UNITDEF" sheetId="5" r:id="rId14"/>
+    <sheet name="Check Type AETB" sheetId="16" r:id="rId15"/>
+    <sheet name="Check Type PGVP" sheetId="15" r:id="rId16"/>
+    <sheet name="Check Type TEST" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13948" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14209" uniqueCount="2119">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -6220,6 +6221,201 @@
   </si>
   <si>
     <t>You did not provide ProviderEmail, which is required for Judd M. Rew.</t>
+  </si>
+  <si>
+    <t>2019-11-07 10</t>
+  </si>
+  <si>
+    <t>QACERT-10-A</t>
+  </si>
+  <si>
+    <t>You reported CompletionTestDate and CompletionTestHour, which is prior to ConditionalBeginDate and ConditionalBeginHour for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "TWCORNEL5-959139C2776D435998D9DF182A3B3DF6"</t>
+  </si>
+  <si>
+    <t>2021-12-20 00</t>
+  </si>
+  <si>
+    <t>QACERT-13-B</t>
+  </si>
+  <si>
+    <t>The RequiredTestCode is not appropriate for the system or component in the event record reported for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-FD2E4272AEF146BDAE361D4E46904B37"</t>
+  </si>
+  <si>
+    <t>QACERT-15-A</t>
+  </si>
+  <si>
+    <t>Based on the EventCode in the record for this event, the certification event requires the following test types: LINE.  However, you have reported a RequiredTestCode that does not include these types of tests.</t>
+  </si>
+  <si>
+    <t>2021-12-27 00</t>
+  </si>
+  <si>
+    <t>QACERT-6-A</t>
+  </si>
+  <si>
+    <t>You reported ConditionalBeginHour but did not report ConditionalBeginDate for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-DEDC606C43184A09AB091D76CFD4DC22"</t>
+  </si>
+  <si>
+    <t>AA1 (SO2)</t>
+  </si>
+  <si>
+    <t>AA6 (SO2)</t>
+  </si>
+  <si>
+    <t>QACERT-8-A</t>
+  </si>
+  <si>
+    <t>You did not provide RequiredTestCode, which is required for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-2EE6184E5D854CB7A271E2842A5640E3"</t>
+  </si>
+  <si>
+    <t>QACERT-4-C</t>
+  </si>
+  <si>
+    <t>Based on the EventDate and EventHour, the monitoring system reported in the event record for this event was not active.</t>
+  </si>
+  <si>
+    <t>QACERT-5-C</t>
+  </si>
+  <si>
+    <t>According to the Monitoring System Component records in the monitoring plan, the component was not active during the event reported in the event record for this event.</t>
+  </si>
+  <si>
+    <t>QACERT-5-A</t>
+  </si>
+  <si>
+    <t>You did not report a ComponentID for this event.  You must provide a ComponentID when the RequiredTestCode indicates that you must perform a component-specific test.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-6392789024C64BA088AF3514D971E883"</t>
+  </si>
+  <si>
+    <t>4000-12-27 00</t>
+  </si>
+  <si>
+    <t>QACERT-2-B</t>
+  </si>
+  <si>
+    <t>You reported a QACertEventDate of 12/27/4000, which is outside the range of acceptable values for this date for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-046E7C9120004C68A61565DD26E93D54"</t>
+  </si>
+  <si>
+    <t>QACERT-12-B</t>
+  </si>
+  <si>
+    <t>The QACertEventCode is not appropriate for the system or component reported in the event record for this event.</t>
+  </si>
+  <si>
+    <t>2006-09-11 06</t>
+  </si>
+  <si>
+    <t>AA9 (FLOW)</t>
+  </si>
+  <si>
+    <t>Based on the EventCode in the record for this event, the certification event requires the following test types: 7DAY.  However, you have reported a RequiredTestCode that does not include these types of tests.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "EPA-C3B62FA230499D0AC987255322B3EF55"</t>
+  </si>
+  <si>
+    <t>2021-12-27 24</t>
+  </si>
+  <si>
+    <t>QACERT-3-B</t>
+  </si>
+  <si>
+    <t>You reported a QACertEventHour of 24, which is outside the range of acceptable values for this hour for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-C6C2C9B494244418A5BB30AC65CF028A"</t>
+  </si>
+  <si>
+    <t>AA8 (CO2)</t>
+  </si>
+  <si>
+    <t>QACERT-9-A</t>
+  </si>
+  <si>
+    <t>You reported ConditionalBeginDate and ConditionalBeginHour, which is prior to QACertEventDate and QACertEventHour for this event.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-7737C2BC0C224390B2A9E78E4ECBEBFA"</t>
+  </si>
+  <si>
+    <t>QACERT-14-G</t>
+  </si>
+  <si>
+    <t>You reported a QA Certification Event record for this event, indicating that this location is an ozone-season-only reporter,  but the Monitor Plan Reporting Frequency records indicate that this location is an annual reporter.</t>
+  </si>
+  <si>
+    <t>Based on the EventCode in the record for this event, the certification event requires the following test types: LINE,RATA.  However, you have reported a RequiredTestCode that does not include these types of tests.</t>
+  </si>
+  <si>
+    <t>QACERT-1-B</t>
+  </si>
+  <si>
+    <t>You reported a QACertEventCode of 99, which requires approval from the EPA.</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-C0E3879920A14159BAA98E03F1980A7A" "CHV-LGIANN-41D6CA4DCB3B4B45AC753004E9D09062"</t>
+  </si>
+  <si>
+    <t>QACERT-7-D</t>
+  </si>
+  <si>
+    <t>You did not report a TestCompletionDate for this event.  If you have not yet completed the tests required for this QA Certification event, you should update the test completion date and hour, and resubmit the record after all tests are completed.</t>
+  </si>
+  <si>
+    <t>Event Code</t>
+  </si>
+  <si>
+    <t>Event Hout</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>2014-10-01 00</t>
+  </si>
+  <si>
+    <t>2015-08-26 08</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-7AA073FE89164FDB9D89D23F2CA36D9C"</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-ED6B3C78DB8946F183CC38BFB172111E"</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-ED705A2D8B5E415B81C4238C224B14CF"</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-45B51BCC6A034B98BAA2D1F58ABDAA71"</t>
+  </si>
+  <si>
+    <t>QCE "TWCORNEL5-F4E3DAADF24B4E1C8F2BEDD2DE59B436" "TWCORNEL5-3F62E109A85942C5803C406C9877D38E"</t>
+  </si>
+  <si>
+    <t>QACERT-16-A</t>
+  </si>
+  <si>
+    <t>A Monitoring Plan associated with this QA certification event has critical errors.  You must correct all active and future Monitoring Plans containing the location in this QA certification event in order to submit this QA certification event to be loaded on EPA's host system.</t>
   </si>
 </sst>
 </file>
@@ -6374,9 +6570,128 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="221">
+  <dxfs count="235">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6440,47 +6755,6 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -7572,125 +7846,145 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="220" dataDxfId="218" headerRowBorderDxfId="219">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}" name="Table9" displayName="Table9" ref="A1:K73" totalsRowShown="0" headerRowDxfId="234" dataDxfId="232" headerRowBorderDxfId="233">
   <autoFilter ref="A1:K73" xr:uid="{5C910FE5-874B-4017-B841-F60367D6DBDE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="217"/>
-    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="216"/>
-    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="215"/>
-    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="214"/>
-    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="213"/>
-    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="212"/>
-    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="211"/>
-    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="210"/>
-    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="209"/>
-    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="208"/>
-    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="207"/>
+    <tableColumn id="1" xr3:uid="{8279D829-3000-4C82-8018-0E78EB4E52ED}" name="Location" dataDxfId="231"/>
+    <tableColumn id="2" xr3:uid="{8C3F4264-2BDD-4183-9522-C40A313B4494}" name="Test Type" dataDxfId="230"/>
+    <tableColumn id="3" xr3:uid="{B0DE5395-DC16-46BB-BC57-85CF8494EEC8}" name="Test Number" dataDxfId="229"/>
+    <tableColumn id="4" xr3:uid="{AFAA091C-FD51-4F17-B61A-9B63F7F60549}" name="Test Date-Time" dataDxfId="228"/>
+    <tableColumn id="5" xr3:uid="{9510359E-2D55-43AD-8BD2-3BEAD6C916CF}" name="Sys/Comp Info" dataDxfId="227"/>
+    <tableColumn id="6" xr3:uid="{AECAE78C-1669-4150-9D54-CF24FB46FB2C}" name="Severity" dataDxfId="226"/>
+    <tableColumn id="7" xr3:uid="{60F04430-453C-4689-B258-ECBB97164B62}" name="EASEY Result Code" dataDxfId="225"/>
+    <tableColumn id="8" xr3:uid="{48BBCC17-5C80-41DD-9F75-59C2F34B310D}" name="Fired" dataDxfId="224"/>
+    <tableColumn id="9" xr3:uid="{B8B66FF4-909C-4ADC-8A89-2420561A8BC8}" name="EASEY Result" dataDxfId="223"/>
+    <tableColumn id="10" xr3:uid="{502F8369-E6BA-4168-9FB1-BDCCFE48BA95}" name="Notes" dataDxfId="222"/>
+    <tableColumn id="11" xr3:uid="{1BA34216-1816-4C5B-91A2-0F623ECC08A9}" name="Command Line Parameters" dataDxfId="221"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
-  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="90"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
+  <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82">
-  <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+  <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="104"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
-  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96">
+  <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="57"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="86"/>
+    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="85"/>
+    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
-  <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82">
+  <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="13">
-  <autoFilter ref="A1:K32" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
+  <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CEF40D72-5DCC-4B34-AFF0-DB646EE7F1D9}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{73E21D38-0138-4A9D-92D7-F5A45463FD70}" name="Test Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F42AD8C2-F06C-4997-B9FA-A329126E0DFF}" name="Test Number" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{854FA5EA-A370-4202-BA3A-9FA3AB721241}" name="Test Date-Time" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{7732B98C-AAD5-4156-A763-0BC4DE759B93}" name="Sys/Comp Info" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{45B5508A-A4AD-4CFF-B677-AD9882050109}" name="Severity" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{C256B736-EB39-4718-8D5D-E6109D13DA65}" name="EASEY Result Code" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{924700DB-01C4-4CC8-9378-33C861B04674}" name="Fired" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{443A7749-F8EE-4346-8DAB-AB037E910CC8}" name="EASEY Result" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{17370406-1790-475D-A379-C70F7A67E837}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{52FD404F-F0C8-42CF-85B7-842E44A87945}" name="Command Line Parameters" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
+  <autoFilter ref="A1:K32" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{CEF40D72-5DCC-4B34-AFF0-DB646EE7F1D9}" name="Location" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{73E21D38-0138-4A9D-92D7-F5A45463FD70}" name="Test Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{F42AD8C2-F06C-4997-B9FA-A329126E0DFF}" name="Test Number" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{854FA5EA-A370-4202-BA3A-9FA3AB721241}" name="Test Date-Time" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{7732B98C-AAD5-4156-A763-0BC4DE759B93}" name="Sys/Comp Info" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{45B5508A-A4AD-4CFF-B677-AD9882050109}" name="Severity" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{C256B736-EB39-4718-8D5D-E6109D13DA65}" name="EASEY Result Code" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{924700DB-01C4-4CC8-9378-33C861B04674}" name="Fired" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{443A7749-F8EE-4346-8DAB-AB037E910CC8}" name="EASEY Result" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{17370406-1790-475D-A379-C70F7A67E837}" name="Notes" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{52FD404F-F0C8-42CF-85B7-842E44A87945}" name="Command Line Parameters" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K26" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}"/>
   <tableColumns count="11">
@@ -7710,7 +8004,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K65" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}"/>
   <tableColumns count="11">
@@ -7731,160 +8025,160 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="206" dataDxfId="204" headerRowBorderDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}" name="Table6" displayName="Table6" ref="A1:K319" totalsRowShown="0" headerRowDxfId="220" dataDxfId="218" headerRowBorderDxfId="219">
   <autoFilter ref="A1:K319" xr:uid="{6E75B64B-AA6D-476A-8302-BF96D5E7E810}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="203"/>
-    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="202"/>
-    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="201"/>
-    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="200"/>
-    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="199"/>
-    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="198"/>
-    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="197"/>
-    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="196"/>
-    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="195"/>
-    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="194"/>
-    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="193"/>
+    <tableColumn id="1" xr3:uid="{DABC54ED-3C28-4B3B-8594-CAA471D265D5}" name="Location" dataDxfId="217"/>
+    <tableColumn id="2" xr3:uid="{F8AEE93E-FDE2-46D7-B1A7-244178C2F820}" name="Test Type" dataDxfId="216"/>
+    <tableColumn id="3" xr3:uid="{8C6E04D8-89F2-453E-9922-8A0AF53CB692}" name="Test Number" dataDxfId="215"/>
+    <tableColumn id="4" xr3:uid="{2B43C86D-8143-4360-87FC-99396C0E304F}" name="Test Date-Time" dataDxfId="214"/>
+    <tableColumn id="5" xr3:uid="{E75FB52D-EC10-43F0-8D77-68CDEA14235D}" name="Sys/Comp Info" dataDxfId="213"/>
+    <tableColumn id="6" xr3:uid="{E6D41DD1-2DAC-4262-AA16-1D46CE14D100}" name="Severity" dataDxfId="212"/>
+    <tableColumn id="7" xr3:uid="{E4B7FCA0-0453-4D46-AF2D-5FCB94154788}" name="EASEY Result Code" dataDxfId="211"/>
+    <tableColumn id="8" xr3:uid="{1C5C127B-0EC6-40C8-9F7F-CDFFB95E2B9C}" name="Fired" dataDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{E4D52144-8081-4E9C-9216-F2B3E7D99696}" name="EASEY Result" dataDxfId="209"/>
+    <tableColumn id="10" xr3:uid="{1B8F57B6-0961-4DCE-A9BB-77E44380F12A}" name="Notes" dataDxfId="208"/>
+    <tableColumn id="11" xr3:uid="{8C749E78-19F9-4D93-A1EC-56160203A547}" name="Command Line Parameters" dataDxfId="207"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}" name="Table11" displayName="Table11" ref="A1:K43" totalsRowShown="0" headerRowDxfId="206" dataDxfId="204" headerRowBorderDxfId="205">
   <autoFilter ref="A1:K43" xr:uid="{D2B13800-7296-41BF-B284-AE9E33207A74}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="188"/>
-    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="185"/>
-    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="184"/>
-    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="183"/>
-    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="182"/>
-    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="181"/>
-    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="180"/>
-    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{5C4086A6-D708-4595-83D3-C24973FA7493}" name="Location" dataDxfId="203"/>
+    <tableColumn id="2" xr3:uid="{85418BD6-CBE3-465C-ABAB-216BDDDEC4AB}" name="Test Type" dataDxfId="202"/>
+    <tableColumn id="3" xr3:uid="{4A0464F8-B583-4C14-9868-15E3FED2D126}" name="Test Number" dataDxfId="201"/>
+    <tableColumn id="4" xr3:uid="{78C8BC19-497D-4CBB-B37C-A591E348A8F4}" name="Test Date-Time" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{1264561D-36B6-4A3C-959A-9E394716E8C7}" name="Sys/Comp Info" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{DD999D52-F401-4681-95E1-7CD8BFBB9B5E}" name="Severity" dataDxfId="198"/>
+    <tableColumn id="7" xr3:uid="{579ED199-5C6A-417A-ADFB-6972029F68D6}" name="EASEY Result Code" dataDxfId="197"/>
+    <tableColumn id="8" xr3:uid="{702EEAA3-DA01-410C-BE7A-D14CFC877E75}" name="Fired" dataDxfId="196"/>
+    <tableColumn id="9" xr3:uid="{DD383C11-E19A-499D-859A-528E10686FA7}" name="EASEY Result" dataDxfId="195"/>
+    <tableColumn id="10" xr3:uid="{C65DEB63-1D14-4EFD-B04E-24DDAC666CD7}" name="Notes" dataDxfId="194"/>
+    <tableColumn id="11" xr3:uid="{F16CC94C-3B79-491F-8B14-14C31351265C}" name="Command Line Parameters" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
-  <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{ADD0CDC3-005A-4908-87CE-24A74B49CF61}" name="Table17" displayName="Table17" ref="A1:K29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:K29" xr:uid="{ADD0CDC3-005A-4908-87CE-24A74B49CF61}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="167"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="166"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="165"/>
+    <tableColumn id="1" xr3:uid="{B56F8537-694B-43C9-A68E-8609AD201C4E}" name="Location" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6DBC46BF-D815-49D3-8182-9348CC54B060}" name="Event Code" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{575144C3-7FC0-46B6-BF5F-2AFF455A12F3}" name="Event Hout" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{9C078E68-941B-436F-8B0A-AC7AEA4D2856}" name="System" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{8AA702CF-37F0-461E-82EF-1D8192AE75F5}" name="Component" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{44FDC991-9A31-45EE-8AFE-7B8A2C3DB067}" name="Severity" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F92E5153-B0F4-49AF-A741-FF7478287E50}" name="EASEY Result Code" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EE2A550F-1ECC-43BA-8D54-2B5A57C82353}" name="Fired" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{BF863843-8882-43DC-9370-234BCBAE2F1E}" name="EASEY Result" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{53139B45-AF9C-4977-B597-D0A55FC6A1BE}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{8B1260FF-BE34-423D-A59F-2DA415AA604B}" name="Command Line Parameters" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="164" headerRowBorderDxfId="163">
-  <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
+  <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="156"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="155"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="154"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="153"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="152"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="186"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="183"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="182"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="181"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="180"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150">
-  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="178" headerRowBorderDxfId="177">
+  <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="176"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="175"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="174"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="173"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="172"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="171"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="170"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="169"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="168"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="167"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
-  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164">
+  <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="128"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="127"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="126"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="125"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="156"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="155"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="154"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="153"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
-  <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150">
+  <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
-  <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
+  <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="98"/>
-    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="126"/>
+    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8190,10 +8484,10 @@
   <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10559,6 +10853,844 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A00A2E-CC49-4E83-9E17-09716099F532}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="133.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="97.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43531.333333333336</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1817</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D3" s="6">
+        <v>43531.333333333336</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D4" s="6">
+        <v>44329.375</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1817</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44329.375</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43531.375</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1825</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="D7" s="6">
+        <v>43531.375</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D8" s="6">
+        <v>44361.375</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D9" s="6">
+        <v>44361.375</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43531.416666666664</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1833</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43531.416666666664</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44329.416666666664</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1837</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44329.416666666664</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43531.458333333336</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1842</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43531.458333333336</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44329.458333333336</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1846</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44329.458333333336</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43553.333333333336</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1851</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43553.333333333336</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="D20" s="6">
+        <v>44341.333333333336</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>1855</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="D21" s="6">
+        <v>44341.333333333336</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="D22" s="6">
+        <v>43555.333333333336</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>1800</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="D23" s="6">
+        <v>43555.333333333336</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="D24" s="6">
+        <v>44341.375</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="D25" s="6">
+        <v>44470.375</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1865</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C84253-C1F3-40A8-BCD6-786B60222E9D}">
   <dimension ref="A1:J68"/>
   <sheetViews>
@@ -10566,7 +11698,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12569,15 +13701,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC7BF0A-744E-4983-9D44-F2CA7F0BDAB9}">
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35:H89"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15191,15 +16323,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF247E8-4CEE-4E4C-AA1C-A5F6418303B4}">
   <dimension ref="A1:K581"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="A1:K1"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33836,15 +34968,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB95806-BA08-44E5-BECF-767BC3A79B45}">
   <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H90" sqref="H90"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36516,15 +37648,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85F61AB-9DA3-44EF-9664-ED9383A7DC6E}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37578,7 +38710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307E8187-44DF-4FB9-8580-48A85C7DC54A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -37586,7 +38718,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:A19"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38448,15 +39580,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D196CC-3DC9-4A6C-BAF4-BA1549D5FF19}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40586,8 +41721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AB6CEE-1A2D-4EDD-BF79-DABF10AD8F60}">
   <dimension ref="A1:K319"/>
   <sheetViews>
-    <sheetView topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="H305" sqref="H305"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52216,14 +53351,977 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD6117F-D81F-4ED3-969D-937806D08C75}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="130.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="38.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="104" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2107</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2108</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2109</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>2118</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="2">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2118</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="2">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>2118</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2">
+        <v>302</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>2118</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="2">
+        <v>311</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>2118</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2054</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>2056</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>2060</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="2">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>2063</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2065</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>2066</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>2071</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2073</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>2076</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>2078</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2073</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2081</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>2082</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>2084</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>2085</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>2060</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="2">
+        <v>300</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2086</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>2088</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B20" s="2">
+        <v>300</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>2091</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>2092</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B21" s="2">
+        <v>300</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>2088</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B22" s="2">
+        <v>800</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>2095</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>2096</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B23" s="2">
+        <v>800</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>2060</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" s="2">
+        <v>800</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2098</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>2099</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" s="2">
+        <v>800</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>2100</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B26" s="2">
+        <v>800</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>2076</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B27" s="2">
+        <v>99</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>2101</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>2102</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B28" s="2">
+        <v>99</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>2060</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B29" s="2">
+        <v>99</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>2105</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1178DED-FAC2-4896-ADA7-BAB067290A3E}">
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53215,15 +55313,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284F8D0C-E6B8-46E4-BE14-B585B6CD2EA0}">
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54150,12 +56248,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A12ED-21A8-440D-BCEA-B358D4E41F2C}">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55464,7 +57562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78B613-4599-4AFD-8861-A9AE5B1FBB5E}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -55472,7 +57570,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56258,7 +58356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F251FFA4-DA4E-420C-9FBD-B96432E43209}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -56266,7 +58364,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57126,842 +59224,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A00A2E-CC49-4E83-9E17-09716099F532}">
-  <dimension ref="A1:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="133.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="45.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="97.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1814</v>
-      </c>
-      <c r="D2" s="6">
-        <v>43531.333333333336</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1815</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1816</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>1817</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1814</v>
-      </c>
-      <c r="D3" s="6">
-        <v>43531.333333333336</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1815</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1820</v>
-      </c>
-      <c r="D4" s="6">
-        <v>44329.375</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1815</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1816</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>1817</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1821</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1820</v>
-      </c>
-      <c r="D5" s="6">
-        <v>44329.375</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1815</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1821</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1822</v>
-      </c>
-      <c r="D6" s="6">
-        <v>43531.375</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1823</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1824</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>1825</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1822</v>
-      </c>
-      <c r="D7" s="6">
-        <v>43531.375</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1823</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D8" s="6">
-        <v>44361.375</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1823</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>1828</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D9" s="6">
-        <v>44361.375</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1823</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1830</v>
-      </c>
-      <c r="D10" s="6">
-        <v>43531.416666666664</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>1832</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>1833</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1830</v>
-      </c>
-      <c r="D11" s="6">
-        <v>43531.416666666664</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1835</v>
-      </c>
-      <c r="D12" s="6">
-        <v>44329.416666666664</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>1836</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>1837</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1835</v>
-      </c>
-      <c r="D13" s="6">
-        <v>44329.416666666664</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1839</v>
-      </c>
-      <c r="D14" s="6">
-        <v>43531.458333333336</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>1841</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>1842</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1839</v>
-      </c>
-      <c r="D15" s="6">
-        <v>43531.458333333336</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D16" s="6">
-        <v>44329.458333333336</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>1845</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>1846</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D17" s="6">
-        <v>44329.458333333336</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1848</v>
-      </c>
-      <c r="D18" s="6">
-        <v>43553.333333333336</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>1849</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>1850</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>1851</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1848</v>
-      </c>
-      <c r="D19" s="6">
-        <v>43553.333333333336</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1849</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>1853</v>
-      </c>
-      <c r="D20" s="6">
-        <v>44341.333333333336</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>1849</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>1854</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>1855</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>1856</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1853</v>
-      </c>
-      <c r="D21" s="6">
-        <v>44341.333333333336</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>1849</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>1856</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1857</v>
-      </c>
-      <c r="D22" s="6">
-        <v>43555.333333333336</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>1859</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>1800</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>1857</v>
-      </c>
-      <c r="D23" s="6">
-        <v>43555.333333333336</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>1861</v>
-      </c>
-      <c r="D24" s="6">
-        <v>44341.375</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>1862</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1863</v>
-      </c>
-      <c r="D25" s="6">
-        <v>44470.375</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>1865</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>1866</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
QCE Testcase additional updates
</commit_message>
<xml_diff>
--- a/misc/Testing Scripts/QA/TestCaseResults.xlsx
+++ b/misc/Testing Scripts/QA/TestCaseResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\CAMDDevelopment\easey-db-scripts\misc\Testing Scripts\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60D5ECC-BD9B-46FB-BD40-5D7AF9FA7D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7249E35-091D-442F-9491-33A92A61E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="809" activeTab="3" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="809" activeTab="3" xr2:uid="{673C86AF-EEEE-433C-9A6E-BD69DDCD2237}"/>
   </bookViews>
   <sheets>
     <sheet name="7DAY" sheetId="9" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14209" uniqueCount="2119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14214" uniqueCount="2119">
   <si>
     <t>ORIS 3 (Barry) Location 5</t>
   </si>
@@ -6571,84 +6571,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="235">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -7602,6 +7524,84 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -7866,159 +7866,159 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}" name="Table12" displayName="Table12" ref="A1:K25" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108">
   <autoFilter ref="A1:K25" xr:uid="{020EA727-A068-4214-96AF-BBB58B4AD2CD}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{17B6DF4E-F31D-42AC-A8A3-2F473C2E30F7}" name="Location" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{1A61DB90-0A47-46E7-8836-10B843CF3280}" name="Test Type" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{C31ACC80-9B40-4B96-9E67-1DC0F8B22187}" name="Test Number" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{80D262AE-185A-4DB8-B5EF-067896A28E0A}" name="Test Date-Time" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{6B683640-6F4D-4D37-B872-927A078A42E7}" name="Sys/Comp Info" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{F2BE968C-9CCB-4176-862E-EA3DBB1F5265}" name="Severity" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{BC1C5663-AD9C-4AF4-8910-56571D431FB2}" name="EASEY Result Code" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{9BDF95D2-C165-45CF-B4F9-D68DB059FCA4}" name="Fired" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{932FF336-A11E-491C-BA6B-0A86BA9E1B8D}" name="EASEY Result" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{DFD2B33B-3898-4612-A48A-7808C887C1CB}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{62C0C95E-EBA4-4A37-A7D6-D1C8B2FB1DD6}" name="Command Line Parameters" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}" name="Table1" displayName="Table1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:J68" xr:uid="{FDFA87AE-4F5C-467B-BD03-84C36AD684CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="105"/>
-    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="104"/>
-    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{4711296A-1683-4D59-9390-9C88803AA68A}" name="Location" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{46A8668E-BFD8-4CE9-8D48-A23DE00E437E}" name="Test Type" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{B7C72E78-CAF2-41A0-B7AC-096EC362072F}" name="Test Number" dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{91E3C101-E9B0-405F-84B0-E044FE40F81E}" name="Test Date-Time" dataDxfId="90"/>
+    <tableColumn id="9" xr3:uid="{D57E3F37-9AD6-40C2-8ACB-5192B0E03191}" name="Sys/Comp Info" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{9415854F-BF69-421C-939D-DB4180DF22DE}" name="Severity" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{5AD12D48-C5A2-4105-B479-271121D42D3E}" name="EASEY Result Code" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{FBEFE9F9-E17E-4E0B-8743-7AE06BE9B114}" name="Fired" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{FCE78312-8A7D-4561-B4CC-F676E43829AF}" name="EASEY Result" dataDxfId="85"/>
+    <tableColumn id="7" xr3:uid="{AA4E3A53-68A9-4DF8-87BC-70FB236A6CED}" name="Notes" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}" name="Table10" displayName="Table10" ref="A1:K89" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82">
   <autoFilter ref="A1:K89" xr:uid="{4A33A717-7F36-46E9-B108-57CE91FC9965}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="89"/>
-    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="88"/>
-    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="87"/>
-    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="85"/>
-    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{CDEE6302-915F-4B8B-8931-C82E789BFD68}" name="Location" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{82F96464-31C7-41F4-99E4-F836EB4804AE}" name="Test Type" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{9A3AD922-1B43-4401-9D08-A69565CBC240}" name="Test Number" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{153B2B1E-9F8A-40A0-9FC6-F154FA69A06D}" name="Test Date-Time" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{EB537EEB-DEA8-4166-A050-FFBFD68D1416}" name="Sys/Comp Info" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{E0692378-248B-472C-9ADE-6DC4C40CE31D}" name="Severity" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{D0B08289-03B0-4D7E-B475-69D81994C3D6}" name="EASEY Result Code" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{8A5BC497-E14C-4A60-9721-3754AC8FBB86}" name="Fired" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{D4027939-C285-4B69-8FE1-5C89204292B8}" name="EASEY Result" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{CAD9076A-ADA1-4DB7-B052-FB52970BED12}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{F61AE4C4-8B02-46C3-94D5-1DAA82EE83BE}" name="Command Line Parameters" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}" name="Table2" displayName="Table2" ref="A1:K581" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
   <autoFilter ref="A1:K581" xr:uid="{12CAFD5A-4B98-4439-A928-885566A8A3A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{2F62CB62-9049-497E-ADC7-F9F96C31FD57}" name="Location" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{4B11ACA0-FDC6-44CA-8A6F-3F08C4CFA5F1}" name="Test Type" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{C41F1DAE-8DC9-48E1-917C-258A6C1E96C9}" name="Test Number" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{EC0CA150-1F20-45D9-9C39-AFA9123777F4}" name="Test Date-Time" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{33FF74A1-9DCC-4D3A-B0C5-64E9380F879C}" name="Sys/Comp Info" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{22A99E8A-A5B5-4CBC-B53D-C1D9D2C5AE1B}" name="Severity" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{029739E6-4C78-4E2E-A09D-8C3FA73D2041}" name="EASEY Result Code" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{5D0E993C-1382-48E9-AA45-BE7DC3BA96AF}" name="Fired" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{F1CFA0F6-70F7-4594-B088-F1D73717D454}" name="EASEY Result" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{40B0439D-9986-4626-9FF3-B32AE7B5EA33}" name="Notes" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{FF29FE95-83D5-44D1-A98E-E38DE83D7BC7}" name="Command Line Parameters" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}" name="Table5" displayName="Table5" ref="A1:K91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
   <autoFilter ref="A1:K91" xr:uid="{72A5AA74-4364-4117-8778-356FF8C70282}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="57"/>
-    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{B5B471E1-992B-4560-9AE9-3A0B01F9D400}" name="Location" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{1012AED6-A79C-434D-9EFD-BC07FE87995E}" name="Test Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{B5631442-9C30-47B5-9E8F-98D77DB400BF}" name="Test Number" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{960A60B0-A29E-44B1-B36A-03ABF8C9387B}" name="Test Date-Time" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{33F281F6-219B-4E02-9434-6B6D946A98E0}" name="Sys/Comp Info" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{E798D1DA-91F4-4F85-BC08-C953E40455E6}" name="Severity" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{D1264FDF-B29D-4FEE-92C2-AB98523233CD}" name="EASEY Result Code" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{C745552B-9704-4998-BE61-D3A91601E678}" name="Fired" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{C834180C-E3EF-4150-9616-ACEC523C5385}" name="EASEY Result" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{3ABD6028-9668-4A63-AEC5-1740A232405E}" name="Notes" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{9F9E58E8-A77F-4D89-A441-47366556DBC4}" name="Command Line Parameters" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
   <autoFilter ref="A1:K32" xr:uid="{AF9DD8BE-C048-408A-9F94-5A8BA21F35EE}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CEF40D72-5DCC-4B34-AFF0-DB646EE7F1D9}" name="Location" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{73E21D38-0138-4A9D-92D7-F5A45463FD70}" name="Test Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{F42AD8C2-F06C-4997-B9FA-A329126E0DFF}" name="Test Number" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{854FA5EA-A370-4202-BA3A-9FA3AB721241}" name="Test Date-Time" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{7732B98C-AAD5-4156-A763-0BC4DE759B93}" name="Sys/Comp Info" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{45B5508A-A4AD-4CFF-B677-AD9882050109}" name="Severity" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{C256B736-EB39-4718-8D5D-E6109D13DA65}" name="EASEY Result Code" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{924700DB-01C4-4CC8-9378-33C861B04674}" name="Fired" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{443A7749-F8EE-4346-8DAB-AB037E910CC8}" name="EASEY Result" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{17370406-1790-475D-A379-C70F7A67E837}" name="Notes" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{52FD404F-F0C8-42CF-85B7-842E44A87945}" name="Command Line Parameters" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{CEF40D72-5DCC-4B34-AFF0-DB646EE7F1D9}" name="Location" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{73E21D38-0138-4A9D-92D7-F5A45463FD70}" name="Test Type" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{F42AD8C2-F06C-4997-B9FA-A329126E0DFF}" name="Test Number" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{854FA5EA-A370-4202-BA3A-9FA3AB721241}" name="Test Date-Time" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{7732B98C-AAD5-4156-A763-0BC4DE759B93}" name="Sys/Comp Info" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{45B5508A-A4AD-4CFF-B677-AD9882050109}" name="Severity" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{C256B736-EB39-4718-8D5D-E6109D13DA65}" name="EASEY Result Code" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{924700DB-01C4-4CC8-9378-33C861B04674}" name="Fired" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{443A7749-F8EE-4346-8DAB-AB037E910CC8}" name="EASEY Result" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{17370406-1790-475D-A379-C70F7A67E837}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{52FD404F-F0C8-42CF-85B7-842E44A87945}" name="Command Line Parameters" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}" name="Table15" displayName="Table15" ref="A1:K26" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
   <autoFilter ref="A1:K26" xr:uid="{F6500E59-5E05-4CE8-8F9D-9221B55D7FD2}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{141A1F22-04AC-41C4-A9F5-CA2D856537D2}" name="Location" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{682EB442-4EFC-4943-86B4-811065481E58}" name="Test Type" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{A5BCB04C-743D-46FA-B0DB-84CF0B6BBC8E}" name="Test Number" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{337B62FF-2ACC-49AF-ACCD-33722D3A358A}" name="Test Date-Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{CA9A9114-48D7-4C09-9D29-E09FD186CBA4}" name="Sys/Comp Info" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{19FB15F6-B8AD-4984-9641-8937F6CFB220}" name="Severity" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{B429ED75-C4D0-4170-8D54-B8270FFB8774}" name="EASEY Result Code" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{B11B957A-B097-47B2-A383-93BC12EF8B7D}" name="Fired" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{C1D59F6D-98B3-4861-AE30-E527BF23B4D6}" name="EASEY Result" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{AF930BC6-6880-489A-BB78-667B6B0662F2}" name="Notes" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{BDA74063-BCCA-4147-84D8-3ACA73246EC1}" name="Command Line Parameters" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{141A1F22-04AC-41C4-A9F5-CA2D856537D2}" name="Location" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{682EB442-4EFC-4943-86B4-811065481E58}" name="Test Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A5BCB04C-743D-46FA-B0DB-84CF0B6BBC8E}" name="Test Number" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{337B62FF-2ACC-49AF-ACCD-33722D3A358A}" name="Test Date-Time" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{CA9A9114-48D7-4C09-9D29-E09FD186CBA4}" name="Sys/Comp Info" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{19FB15F6-B8AD-4984-9641-8937F6CFB220}" name="Severity" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{B429ED75-C4D0-4170-8D54-B8270FFB8774}" name="EASEY Result Code" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{B11B957A-B097-47B2-A383-93BC12EF8B7D}" name="Fired" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{C1D59F6D-98B3-4861-AE30-E527BF23B4D6}" name="EASEY Result" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{AF930BC6-6880-489A-BB78-667B6B0662F2}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{BDA74063-BCCA-4147-84D8-3ACA73246EC1}" name="Command Line Parameters" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}" name="Table14" displayName="Table14" ref="A1:K65" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
   <autoFilter ref="A1:K65" xr:uid="{4A6B4518-3730-4EDB-8118-7FC685E54D4D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{688BE455-22E7-460C-AEB8-77FED1C57AE3}" name="Location" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{20C8F268-F0DA-4C4B-85CC-9675F4020B20}" name="Test Type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{54552E71-F736-4EBF-B675-B592F1FEB306}" name="Test Number" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{AE42C9A1-5DFB-4CAB-8EF8-07F76F7C7F72}" name="Test Date-Time" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{59716E11-5EC0-4CF7-9C60-46F006BF4A88}" name="Sys/Comp Info" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{C2858AAF-8CC6-49B5-8987-6A43E1C7AE69}" name="Severity" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{A0BA8D72-C986-43E0-A3BB-DFA920174AFC}" name="EASEY Result Code" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{39E9C69F-1E34-4D36-B7C3-F2D6A86BBD74}" name="Fired" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{ACAE356B-0C07-4041-B1FC-2027B441EF49}" name="EASEY Result" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{356D670A-5642-493A-B84F-2CC68F64CC3B}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{B4F1D6ED-902F-4D6E-967E-05C2040CB5E8}" name="Command Line Parameters" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8065,120 +8065,120 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{ADD0CDC3-005A-4908-87CE-24A74B49CF61}" name="Table17" displayName="Table17" ref="A1:K29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{ADD0CDC3-005A-4908-87CE-24A74B49CF61}" name="Table17" displayName="Table17" ref="A1:K29" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
   <autoFilter ref="A1:K29" xr:uid="{ADD0CDC3-005A-4908-87CE-24A74B49CF61}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B56F8537-694B-43C9-A68E-8609AD201C4E}" name="Location" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{6DBC46BF-D815-49D3-8182-9348CC54B060}" name="Event Code" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{575144C3-7FC0-46B6-BF5F-2AFF455A12F3}" name="Event Hout" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{9C078E68-941B-436F-8B0A-AC7AEA4D2856}" name="System" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{8AA702CF-37F0-461E-82EF-1D8192AE75F5}" name="Component" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{44FDC991-9A31-45EE-8AFE-7B8A2C3DB067}" name="Severity" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F92E5153-B0F4-49AF-A741-FF7478287E50}" name="EASEY Result Code" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{EE2A550F-1ECC-43BA-8D54-2B5A57C82353}" name="Fired" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{BF863843-8882-43DC-9370-234BCBAE2F1E}" name="EASEY Result" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{53139B45-AF9C-4977-B597-D0A55FC6A1BE}" name="Notes" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{8B1260FF-BE34-423D-A59F-2DA415AA604B}" name="Command Line Parameters" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B56F8537-694B-43C9-A68E-8609AD201C4E}" name="Location" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{6DBC46BF-D815-49D3-8182-9348CC54B060}" name="Event Code" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{575144C3-7FC0-46B6-BF5F-2AFF455A12F3}" name="Event Hout" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{9C078E68-941B-436F-8B0A-AC7AEA4D2856}" name="System" dataDxfId="186"/>
+    <tableColumn id="5" xr3:uid="{8AA702CF-37F0-461E-82EF-1D8192AE75F5}" name="Component" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{44FDC991-9A31-45EE-8AFE-7B8A2C3DB067}" name="Severity" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{F92E5153-B0F4-49AF-A741-FF7478287E50}" name="EASEY Result Code" dataDxfId="183"/>
+    <tableColumn id="8" xr3:uid="{EE2A550F-1ECC-43BA-8D54-2B5A57C82353}" name="Fired" dataDxfId="182"/>
+    <tableColumn id="9" xr3:uid="{BF863843-8882-43DC-9370-234BCBAE2F1E}" name="EASEY Result" dataDxfId="181"/>
+    <tableColumn id="10" xr3:uid="{53139B45-AF9C-4977-B597-D0A55FC6A1BE}" name="Notes" dataDxfId="180"/>
+    <tableColumn id="11" xr3:uid="{8B1260FF-BE34-423D-A59F-2DA415AA604B}" name="Command Line Parameters" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}" name="Table7" displayName="Table7" ref="A1:K33" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177">
   <autoFilter ref="A1:K33" xr:uid="{643FA4C3-7226-4FC1-A77A-D6CF46B7DE06}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="188"/>
-    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="185"/>
-    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="184"/>
-    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="183"/>
-    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="182"/>
-    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="181"/>
-    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="180"/>
-    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{6A1DC097-B550-4298-811F-BB553C8A78B7}" name="Location" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{B0B911C5-C9AF-4D6B-9A8E-E4524ABB1455}" name="Test Type" dataDxfId="174"/>
+    <tableColumn id="3" xr3:uid="{7C46186D-C3D8-4F3A-A359-DBEC33D11A32}" name="Test Number" dataDxfId="173"/>
+    <tableColumn id="4" xr3:uid="{B77DADA4-D1C0-49A5-8941-BF36C2738914}" name="Test Date-Time" dataDxfId="172"/>
+    <tableColumn id="5" xr3:uid="{94D2842C-7497-4826-BFDF-64C1F4930DC7}" name="Sys/Comp Info" dataDxfId="171"/>
+    <tableColumn id="6" xr3:uid="{18E0026A-3AB3-4471-BB8D-F86CD1FCACB2}" name="Severity" dataDxfId="170"/>
+    <tableColumn id="7" xr3:uid="{64F844FE-3B1B-48BD-BFA3-F73DD8F6BAE7}" name="EASEY Result Code" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{0A777F6A-C367-4D68-80DC-BE82994A6C9C}" name="Fired" dataDxfId="168"/>
+    <tableColumn id="9" xr3:uid="{58E8A6A7-2EB9-4636-98D8-915BAA276364}" name="EASEY Result" dataDxfId="167"/>
+    <tableColumn id="10" xr3:uid="{8E16DEBD-9C74-43B0-A1EC-12CF584BC57D}" name="Notes" dataDxfId="166"/>
+    <tableColumn id="11" xr3:uid="{7AE3F542-B6CD-45CB-99F0-47DDE95004F7}" name="Command Line Parameters" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="178" headerRowBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}" name="Table8" displayName="Table8" ref="A1:K28" totalsRowShown="0" headerRowDxfId="164" headerRowBorderDxfId="163">
   <autoFilter ref="A1:K28" xr:uid="{E4484FF7-4E72-42BE-B673-2211F40DBEC5}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="176"/>
-    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="175"/>
-    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="174"/>
-    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="173"/>
-    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="172"/>
-    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="171"/>
-    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="170"/>
-    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="169"/>
-    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="168"/>
-    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="167"/>
-    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="166"/>
+    <tableColumn id="1" xr3:uid="{BCDEC250-D556-489B-A8C0-F3C0B749EE85}" name="Location" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{27845E29-DF76-4FC1-8B99-E6D05BC504AB}" name="Test Type" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{88E8B5E9-3A4F-487A-A1FD-2F8825130F6C}" name="Test Number" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{96597CE9-7403-4439-ACB1-4DB48A5AE831}" name="Test Date-Time" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{67D38623-BE59-4D0E-966A-D900405266E4}" name="Sys/Comp Info" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{4480DA93-63BE-46D7-9C44-A62CF4C30DB9}" name="Severity" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{4DE029FD-1894-4C16-A49E-7205888520D7}" name="EASEY Result Code" dataDxfId="156"/>
+    <tableColumn id="8" xr3:uid="{38E45A86-E2E8-436C-83B0-1DC52A25A389}" name="Fired" dataDxfId="155"/>
+    <tableColumn id="9" xr3:uid="{D0FCA1F1-B5E4-4F39-8570-3FDAAFD8C655}" name="EASEY Result" dataDxfId="154"/>
+    <tableColumn id="10" xr3:uid="{8FFB2F06-8DA3-4256-9B20-894A86F3CAB1}" name="Notes" dataDxfId="153"/>
+    <tableColumn id="11" xr3:uid="{0A82F04A-4DC9-465C-ACBF-8A9107DE5BF9}" name="Command Line Parameters" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}" name="Table4" displayName="Table4" ref="A1:K44" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150">
   <autoFilter ref="A1:K44" xr:uid="{C4E4C8FF-D2BC-4023-A7E2-4F0FE1340DDB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="156"/>
-    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="155"/>
-    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="154"/>
-    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="153"/>
-    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="152"/>
+    <tableColumn id="1" xr3:uid="{25672079-CDA0-4D8B-8CF3-D545B2ACD419}" name="Location" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{5279C203-946F-4765-ABB9-8C81921C2DC3}" name="Test Type" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{11DE1298-C62C-4C4B-9989-25AA10EF10C0}" name="Test Number" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{2A458B2D-9FF3-4418-9FD6-DF0766209CB5}" name="Test Date-Time" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{60E36B10-857E-4482-B035-790F74DBDB33}" name="Sys/Comp Info" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{2E26423A-D6BE-4410-8F61-F74A3CED15B8}" name="Severity" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{20497C37-19CA-4417-AC58-9CBBEB217149}" name="EASEY Result Code" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{B51DBED3-688D-4748-9F71-406904878E83}" name="Fired" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{55BF46DF-A688-44E7-9212-0315C9101E05}" name="EASEY Result" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{A4FC5CC8-E769-426F-AEEE-D8BDE3AAE1AB}" name="Notes" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{E7F09088-0589-40C2-8067-9D1FE0896663}" name="Command Line Parameters" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}" name="Table3" displayName="Table3" ref="A1:K26" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
   <autoFilter ref="A1:K26" xr:uid="{0CC4DB58-871D-4311-83EC-9DB6A2F24D3C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{FD39BA7F-4A73-45B6-8492-9C47A87EAF80}" name="Location" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{6BD18705-A907-480B-9613-FD6A89008B95}" name="Test Type" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{171EC70D-BD2B-4679-9E2F-B7A72F41A5BC}" name="Test Number" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{54392DF7-D2E8-406A-BF46-C94A6AF058B7}" name="Test Date-Time" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{BEE30332-3FC4-42CC-9E0A-10D6FD8CE7DB}" name="Sys/Comp Info" dataDxfId="130"/>
+    <tableColumn id="6" xr3:uid="{4D56506A-EEFD-4953-B5C2-BFBFB1100C42}" name="Severity" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{F7744816-5978-4331-B8B7-FBAEA071B23C}" name="EASEY Result Code" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{5A8FF3A4-DEAC-4772-A7B5-657662710593}" name="Fired" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{B72C4A8D-A7B2-492D-AAF3-C53B34CC6D68}" name="EASEY Result" dataDxfId="126"/>
+    <tableColumn id="10" xr3:uid="{3BD58939-520E-4EF9-ACA2-F4F2053AAB3E}" name="Notes" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{81440B9B-FEDA-4EF7-8E5F-058F42001F39}" name="Command Line Parameters" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="137" dataDxfId="135" headerRowBorderDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}" name="Table13" displayName="Table13" ref="A1:K26" totalsRowShown="0" headerRowDxfId="123" dataDxfId="121" headerRowBorderDxfId="122">
   <autoFilter ref="A1:K26" xr:uid="{387CD9B0-42DD-43F6-B933-FC392A3DA7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="132"/>
-    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="129"/>
-    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="128"/>
-    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="127"/>
-    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="126"/>
-    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="125"/>
-    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{58A7C390-8DB8-4C87-940A-55AE4A3592FC}" name="Location" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{A3FC97A4-B761-48C4-BB4C-19DA9785E4DF}" name="Test Type" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{3A3BD58D-EB20-4F67-8215-8A96EE69C978}" name="Test Number" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{DE80CD30-41D0-4B53-8DE7-4F269F701558}" name="Test Date-Time" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{B86A2D2D-C8EB-483C-BF81-EB9D9F4E66F2}" name="Sys/Comp Info" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{36B980F4-27FC-477D-A50F-623E7E0A94DE}" name="Severity" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{A9D38791-49D7-4EB3-896C-646601058179}" name="EASEY Result Code" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{938968FB-CC01-4403-A09B-C4F6161B5D90}" name="Fired" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{25329D8A-5A94-4418-84D8-82518A7923BD}" name="EASEY Result" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{D60A5A6A-A087-4FC2-96A5-060A26AA48C8}" name="Notes" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{5DE715B2-E8F2-48F0-9DE2-694E23DB23E9}" name="Command Line Parameters" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -39588,10 +39588,10 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53361,7 +53361,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:H6"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53375,7 +53375,7 @@
     <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="130.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="38.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="75.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="104" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -53415,7 +53415,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
@@ -53443,11 +53443,14 @@
       <c r="I2" s="5" t="s">
         <v>2118</v>
       </c>
+      <c r="J2" s="16" t="s">
+        <v>1987</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>2112</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -53475,11 +53478,14 @@
       <c r="I3" s="5" t="s">
         <v>2118</v>
       </c>
+      <c r="J3" s="16" t="s">
+        <v>1987</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>2113</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -53507,11 +53513,14 @@
       <c r="I4" s="5" t="s">
         <v>2118</v>
       </c>
+      <c r="J4" s="16" t="s">
+        <v>1987</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>2114</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>108</v>
       </c>
@@ -53539,11 +53548,14 @@
       <c r="I5" s="5" t="s">
         <v>2118</v>
       </c>
+      <c r="J5" s="16" t="s">
+        <v>1987</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>2115</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -53570,6 +53582,9 @@
       </c>
       <c r="I6" s="5" t="s">
         <v>2118</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>1987</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>2116</v>
@@ -56079,7 +56094,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>1299</v>
       </c>
@@ -56111,7 +56126,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>1299</v>
       </c>
@@ -59122,7 +59137,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1202</v>
       </c>

</xml_diff>